<commit_message>
Modify network to use 2x2 pooling only
</commit_message>
<xml_diff>
--- a/ai84net.xlsx
+++ b/ai84net.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert.muchsel/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert.muchsel/Documents/Source/ai84/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910DF67C-7001-B84D-8DA7-3D3CBB27D0A5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F3967B-75FE-8342-83FF-331EA4BB4149}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10360" yWindow="460" windowWidth="40140" windowHeight="27200" xr2:uid="{F7B6694D-E61F-7A45-81C3-7DF16BE80F2B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="40">
   <si>
     <t>conv1</t>
   </si>
@@ -142,6 +142,15 @@
   </si>
   <si>
     <t>GROUP 3</t>
+  </si>
+  <si>
+    <t>mp+conv2</t>
+  </si>
+  <si>
+    <t>mp+conv3</t>
+  </si>
+  <si>
+    <t>ap+conv4</t>
   </si>
 </sst>
 </file>
@@ -898,6 +907,66 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -916,72 +985,12 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1591,7 +1600,7 @@
   <dimension ref="A1:EB91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="DQ11" sqref="DQ11"/>
+      <selection activeCell="BV88" sqref="BV88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2126,7 +2135,7 @@
       </c>
     </row>
     <row r="3" spans="1:130" ht="17" thickBot="1">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="112" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="83">
@@ -2194,7 +2203,7 @@
       <c r="BH3" s="7"/>
       <c r="BI3" s="7"/>
       <c r="BJ3" s="9"/>
-      <c r="BK3" s="110"/>
+      <c r="BK3" s="86"/>
       <c r="BL3" s="10"/>
       <c r="BM3" s="10"/>
       <c r="BN3" s="10"/>
@@ -2264,12 +2273,12 @@
       <c r="DZ3" s="11"/>
     </row>
     <row r="4" spans="1:130">
-      <c r="A4" s="87"/>
+      <c r="A4" s="113"/>
       <c r="B4" s="84">
         <f>B3+1</f>
         <v>1</v>
       </c>
-      <c r="C4" s="111"/>
+      <c r="C4" s="87"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -2329,347 +2338,347 @@
       <c r="BH4" s="12"/>
       <c r="BI4" s="12"/>
       <c r="BJ4" s="12"/>
-      <c r="BK4" s="112"/>
-      <c r="BL4" s="112"/>
-      <c r="BM4" s="112"/>
-      <c r="BN4" s="112"/>
-      <c r="BO4" s="112"/>
-      <c r="BP4" s="112"/>
-      <c r="BQ4" s="112"/>
-      <c r="BR4" s="112"/>
-      <c r="BS4" s="112"/>
-      <c r="BT4" s="112"/>
-      <c r="BU4" s="112"/>
-      <c r="BV4" s="112"/>
-      <c r="BW4" s="112"/>
-      <c r="BX4" s="112"/>
-      <c r="BY4" s="112"/>
-      <c r="BZ4" s="112"/>
-      <c r="CA4" s="112"/>
-      <c r="CB4" s="112"/>
-      <c r="CC4" s="112"/>
-      <c r="CD4" s="112"/>
-      <c r="CE4" s="112"/>
-      <c r="CF4" s="112"/>
-      <c r="CG4" s="112"/>
-      <c r="CH4" s="112"/>
-      <c r="CI4" s="112"/>
-      <c r="CJ4" s="112"/>
-      <c r="CK4" s="112"/>
-      <c r="CL4" s="112"/>
-      <c r="CM4" s="112"/>
-      <c r="CN4" s="112"/>
-      <c r="CO4" s="112"/>
-      <c r="CP4" s="112"/>
-      <c r="CQ4" s="112"/>
-      <c r="CR4" s="112"/>
-      <c r="CS4" s="112"/>
-      <c r="CT4" s="112"/>
-      <c r="CU4" s="112"/>
-      <c r="CV4" s="112"/>
-      <c r="CW4" s="112"/>
-      <c r="CX4" s="112"/>
-      <c r="CY4" s="112"/>
-      <c r="CZ4" s="112"/>
-      <c r="DA4" s="112"/>
-      <c r="DB4" s="112"/>
-      <c r="DC4" s="112"/>
-      <c r="DD4" s="112"/>
-      <c r="DE4" s="112"/>
-      <c r="DF4" s="112"/>
-      <c r="DG4" s="112"/>
-      <c r="DH4" s="112"/>
-      <c r="DI4" s="112"/>
-      <c r="DJ4" s="112"/>
-      <c r="DK4" s="112"/>
-      <c r="DL4" s="112"/>
-      <c r="DM4" s="112"/>
-      <c r="DN4" s="112"/>
-      <c r="DO4" s="112"/>
-      <c r="DP4" s="112"/>
-      <c r="DQ4" s="112"/>
-      <c r="DR4" s="112"/>
-      <c r="DS4" s="112"/>
-      <c r="DT4" s="112"/>
-      <c r="DU4" s="112"/>
-      <c r="DV4" s="112"/>
-      <c r="DW4" s="112"/>
-      <c r="DX4" s="112"/>
-      <c r="DY4" s="112"/>
-      <c r="DZ4" s="113"/>
+      <c r="BK4" s="88"/>
+      <c r="BL4" s="88"/>
+      <c r="BM4" s="88"/>
+      <c r="BN4" s="88"/>
+      <c r="BO4" s="88"/>
+      <c r="BP4" s="88"/>
+      <c r="BQ4" s="88"/>
+      <c r="BR4" s="88"/>
+      <c r="BS4" s="88"/>
+      <c r="BT4" s="88"/>
+      <c r="BU4" s="88"/>
+      <c r="BV4" s="88"/>
+      <c r="BW4" s="88"/>
+      <c r="BX4" s="88"/>
+      <c r="BY4" s="88"/>
+      <c r="BZ4" s="88"/>
+      <c r="CA4" s="88"/>
+      <c r="CB4" s="88"/>
+      <c r="CC4" s="88"/>
+      <c r="CD4" s="88"/>
+      <c r="CE4" s="88"/>
+      <c r="CF4" s="88"/>
+      <c r="CG4" s="88"/>
+      <c r="CH4" s="88"/>
+      <c r="CI4" s="88"/>
+      <c r="CJ4" s="88"/>
+      <c r="CK4" s="88"/>
+      <c r="CL4" s="88"/>
+      <c r="CM4" s="88"/>
+      <c r="CN4" s="88"/>
+      <c r="CO4" s="88"/>
+      <c r="CP4" s="88"/>
+      <c r="CQ4" s="88"/>
+      <c r="CR4" s="88"/>
+      <c r="CS4" s="88"/>
+      <c r="CT4" s="88"/>
+      <c r="CU4" s="88"/>
+      <c r="CV4" s="88"/>
+      <c r="CW4" s="88"/>
+      <c r="CX4" s="88"/>
+      <c r="CY4" s="88"/>
+      <c r="CZ4" s="88"/>
+      <c r="DA4" s="88"/>
+      <c r="DB4" s="88"/>
+      <c r="DC4" s="88"/>
+      <c r="DD4" s="88"/>
+      <c r="DE4" s="88"/>
+      <c r="DF4" s="88"/>
+      <c r="DG4" s="88"/>
+      <c r="DH4" s="88"/>
+      <c r="DI4" s="88"/>
+      <c r="DJ4" s="88"/>
+      <c r="DK4" s="88"/>
+      <c r="DL4" s="88"/>
+      <c r="DM4" s="88"/>
+      <c r="DN4" s="88"/>
+      <c r="DO4" s="88"/>
+      <c r="DP4" s="88"/>
+      <c r="DQ4" s="88"/>
+      <c r="DR4" s="88"/>
+      <c r="DS4" s="88"/>
+      <c r="DT4" s="88"/>
+      <c r="DU4" s="88"/>
+      <c r="DV4" s="88"/>
+      <c r="DW4" s="88"/>
+      <c r="DX4" s="88"/>
+      <c r="DY4" s="88"/>
+      <c r="DZ4" s="89"/>
     </row>
     <row r="5" spans="1:130">
-      <c r="A5" s="87"/>
+      <c r="A5" s="113"/>
       <c r="B5" s="84">
         <f t="shared" ref="B5:B66" si="1">B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="114"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="112"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="112"/>
-      <c r="K5" s="112"/>
-      <c r="L5" s="112"/>
-      <c r="M5" s="112"/>
-      <c r="N5" s="112"/>
-      <c r="O5" s="112"/>
-      <c r="P5" s="112"/>
-      <c r="Q5" s="112"/>
-      <c r="R5" s="112"/>
-      <c r="S5" s="112"/>
-      <c r="T5" s="112"/>
-      <c r="U5" s="112"/>
-      <c r="V5" s="112"/>
-      <c r="W5" s="112"/>
-      <c r="X5" s="112"/>
-      <c r="Y5" s="112"/>
-      <c r="Z5" s="112"/>
-      <c r="AA5" s="112"/>
-      <c r="AB5" s="112"/>
-      <c r="AC5" s="112"/>
-      <c r="AD5" s="112"/>
-      <c r="AE5" s="112"/>
-      <c r="AF5" s="112"/>
-      <c r="AG5" s="112"/>
-      <c r="AH5" s="112"/>
-      <c r="AI5" s="112"/>
-      <c r="AJ5" s="112"/>
-      <c r="AK5" s="112"/>
-      <c r="AL5" s="112"/>
-      <c r="AM5" s="112"/>
-      <c r="AN5" s="112"/>
-      <c r="AO5" s="112"/>
-      <c r="AP5" s="112"/>
-      <c r="AQ5" s="112"/>
-      <c r="AR5" s="112"/>
-      <c r="AS5" s="112"/>
-      <c r="AT5" s="112"/>
-      <c r="AU5" s="112"/>
-      <c r="AV5" s="112"/>
-      <c r="AW5" s="112"/>
-      <c r="AX5" s="112"/>
-      <c r="AY5" s="112"/>
-      <c r="AZ5" s="112"/>
-      <c r="BA5" s="112"/>
-      <c r="BB5" s="112"/>
-      <c r="BC5" s="112"/>
-      <c r="BD5" s="112"/>
-      <c r="BE5" s="112"/>
-      <c r="BF5" s="112"/>
-      <c r="BG5" s="112"/>
-      <c r="BH5" s="112"/>
-      <c r="BI5" s="112"/>
-      <c r="BJ5" s="112"/>
-      <c r="BK5" s="112"/>
-      <c r="BL5" s="112"/>
-      <c r="BM5" s="112"/>
-      <c r="BN5" s="112"/>
-      <c r="BO5" s="112"/>
-      <c r="BP5" s="112"/>
-      <c r="BQ5" s="112"/>
-      <c r="BR5" s="112"/>
-      <c r="BS5" s="112"/>
-      <c r="BT5" s="112"/>
-      <c r="BU5" s="112"/>
-      <c r="BV5" s="112"/>
-      <c r="BW5" s="112"/>
-      <c r="BX5" s="112"/>
-      <c r="BY5" s="112"/>
-      <c r="BZ5" s="112"/>
-      <c r="CA5" s="112"/>
-      <c r="CB5" s="112"/>
-      <c r="CC5" s="112"/>
-      <c r="CD5" s="112"/>
-      <c r="CE5" s="112"/>
-      <c r="CF5" s="112"/>
-      <c r="CG5" s="112"/>
-      <c r="CH5" s="112"/>
-      <c r="CI5" s="112"/>
-      <c r="CJ5" s="112"/>
-      <c r="CK5" s="112"/>
-      <c r="CL5" s="112"/>
-      <c r="CM5" s="112"/>
-      <c r="CN5" s="112"/>
-      <c r="CO5" s="112"/>
-      <c r="CP5" s="112"/>
-      <c r="CQ5" s="112"/>
-      <c r="CR5" s="112"/>
-      <c r="CS5" s="112"/>
-      <c r="CT5" s="112"/>
-      <c r="CU5" s="112"/>
-      <c r="CV5" s="112"/>
-      <c r="CW5" s="112"/>
-      <c r="CX5" s="112"/>
-      <c r="CY5" s="112"/>
-      <c r="CZ5" s="112"/>
-      <c r="DA5" s="112"/>
-      <c r="DB5" s="112"/>
-      <c r="DC5" s="112"/>
-      <c r="DD5" s="112"/>
-      <c r="DE5" s="112"/>
-      <c r="DF5" s="112"/>
-      <c r="DG5" s="112"/>
-      <c r="DH5" s="112"/>
-      <c r="DI5" s="112"/>
-      <c r="DJ5" s="112"/>
-      <c r="DK5" s="112"/>
-      <c r="DL5" s="112"/>
-      <c r="DM5" s="112"/>
-      <c r="DN5" s="112"/>
-      <c r="DO5" s="112"/>
-      <c r="DP5" s="112"/>
-      <c r="DQ5" s="112"/>
-      <c r="DR5" s="112"/>
-      <c r="DS5" s="112"/>
-      <c r="DT5" s="112"/>
-      <c r="DU5" s="112"/>
-      <c r="DV5" s="112"/>
-      <c r="DW5" s="112"/>
-      <c r="DX5" s="112"/>
-      <c r="DY5" s="112"/>
-      <c r="DZ5" s="113"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="88"/>
+      <c r="M5" s="88"/>
+      <c r="N5" s="88"/>
+      <c r="O5" s="88"/>
+      <c r="P5" s="88"/>
+      <c r="Q5" s="88"/>
+      <c r="R5" s="88"/>
+      <c r="S5" s="88"/>
+      <c r="T5" s="88"/>
+      <c r="U5" s="88"/>
+      <c r="V5" s="88"/>
+      <c r="W5" s="88"/>
+      <c r="X5" s="88"/>
+      <c r="Y5" s="88"/>
+      <c r="Z5" s="88"/>
+      <c r="AA5" s="88"/>
+      <c r="AB5" s="88"/>
+      <c r="AC5" s="88"/>
+      <c r="AD5" s="88"/>
+      <c r="AE5" s="88"/>
+      <c r="AF5" s="88"/>
+      <c r="AG5" s="88"/>
+      <c r="AH5" s="88"/>
+      <c r="AI5" s="88"/>
+      <c r="AJ5" s="88"/>
+      <c r="AK5" s="88"/>
+      <c r="AL5" s="88"/>
+      <c r="AM5" s="88"/>
+      <c r="AN5" s="88"/>
+      <c r="AO5" s="88"/>
+      <c r="AP5" s="88"/>
+      <c r="AQ5" s="88"/>
+      <c r="AR5" s="88"/>
+      <c r="AS5" s="88"/>
+      <c r="AT5" s="88"/>
+      <c r="AU5" s="88"/>
+      <c r="AV5" s="88"/>
+      <c r="AW5" s="88"/>
+      <c r="AX5" s="88"/>
+      <c r="AY5" s="88"/>
+      <c r="AZ5" s="88"/>
+      <c r="BA5" s="88"/>
+      <c r="BB5" s="88"/>
+      <c r="BC5" s="88"/>
+      <c r="BD5" s="88"/>
+      <c r="BE5" s="88"/>
+      <c r="BF5" s="88"/>
+      <c r="BG5" s="88"/>
+      <c r="BH5" s="88"/>
+      <c r="BI5" s="88"/>
+      <c r="BJ5" s="88"/>
+      <c r="BK5" s="88"/>
+      <c r="BL5" s="88"/>
+      <c r="BM5" s="88"/>
+      <c r="BN5" s="88"/>
+      <c r="BO5" s="88"/>
+      <c r="BP5" s="88"/>
+      <c r="BQ5" s="88"/>
+      <c r="BR5" s="88"/>
+      <c r="BS5" s="88"/>
+      <c r="BT5" s="88"/>
+      <c r="BU5" s="88"/>
+      <c r="BV5" s="88"/>
+      <c r="BW5" s="88"/>
+      <c r="BX5" s="88"/>
+      <c r="BY5" s="88"/>
+      <c r="BZ5" s="88"/>
+      <c r="CA5" s="88"/>
+      <c r="CB5" s="88"/>
+      <c r="CC5" s="88"/>
+      <c r="CD5" s="88"/>
+      <c r="CE5" s="88"/>
+      <c r="CF5" s="88"/>
+      <c r="CG5" s="88"/>
+      <c r="CH5" s="88"/>
+      <c r="CI5" s="88"/>
+      <c r="CJ5" s="88"/>
+      <c r="CK5" s="88"/>
+      <c r="CL5" s="88"/>
+      <c r="CM5" s="88"/>
+      <c r="CN5" s="88"/>
+      <c r="CO5" s="88"/>
+      <c r="CP5" s="88"/>
+      <c r="CQ5" s="88"/>
+      <c r="CR5" s="88"/>
+      <c r="CS5" s="88"/>
+      <c r="CT5" s="88"/>
+      <c r="CU5" s="88"/>
+      <c r="CV5" s="88"/>
+      <c r="CW5" s="88"/>
+      <c r="CX5" s="88"/>
+      <c r="CY5" s="88"/>
+      <c r="CZ5" s="88"/>
+      <c r="DA5" s="88"/>
+      <c r="DB5" s="88"/>
+      <c r="DC5" s="88"/>
+      <c r="DD5" s="88"/>
+      <c r="DE5" s="88"/>
+      <c r="DF5" s="88"/>
+      <c r="DG5" s="88"/>
+      <c r="DH5" s="88"/>
+      <c r="DI5" s="88"/>
+      <c r="DJ5" s="88"/>
+      <c r="DK5" s="88"/>
+      <c r="DL5" s="88"/>
+      <c r="DM5" s="88"/>
+      <c r="DN5" s="88"/>
+      <c r="DO5" s="88"/>
+      <c r="DP5" s="88"/>
+      <c r="DQ5" s="88"/>
+      <c r="DR5" s="88"/>
+      <c r="DS5" s="88"/>
+      <c r="DT5" s="88"/>
+      <c r="DU5" s="88"/>
+      <c r="DV5" s="88"/>
+      <c r="DW5" s="88"/>
+      <c r="DX5" s="88"/>
+      <c r="DY5" s="88"/>
+      <c r="DZ5" s="89"/>
     </row>
     <row r="6" spans="1:130" ht="17" thickBot="1">
-      <c r="A6" s="87"/>
+      <c r="A6" s="113"/>
       <c r="B6" s="84">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="116"/>
-      <c r="E6" s="116"/>
-      <c r="F6" s="116"/>
-      <c r="G6" s="116"/>
-      <c r="H6" s="116"/>
-      <c r="I6" s="116"/>
-      <c r="J6" s="116"/>
-      <c r="K6" s="116"/>
-      <c r="L6" s="116"/>
-      <c r="M6" s="116"/>
-      <c r="N6" s="116"/>
-      <c r="O6" s="116"/>
-      <c r="P6" s="116"/>
-      <c r="Q6" s="116"/>
-      <c r="R6" s="116"/>
-      <c r="S6" s="116"/>
-      <c r="T6" s="116"/>
-      <c r="U6" s="116"/>
-      <c r="V6" s="116"/>
-      <c r="W6" s="116"/>
-      <c r="X6" s="116"/>
-      <c r="Y6" s="116"/>
-      <c r="Z6" s="116"/>
-      <c r="AA6" s="116"/>
-      <c r="AB6" s="116"/>
-      <c r="AC6" s="116"/>
-      <c r="AD6" s="116"/>
-      <c r="AE6" s="116"/>
-      <c r="AF6" s="116"/>
-      <c r="AG6" s="116"/>
-      <c r="AH6" s="116"/>
-      <c r="AI6" s="116"/>
-      <c r="AJ6" s="116"/>
-      <c r="AK6" s="116"/>
-      <c r="AL6" s="116"/>
-      <c r="AM6" s="116"/>
-      <c r="AN6" s="116"/>
-      <c r="AO6" s="116"/>
-      <c r="AP6" s="116"/>
-      <c r="AQ6" s="116"/>
-      <c r="AR6" s="116"/>
-      <c r="AS6" s="116"/>
-      <c r="AT6" s="116"/>
-      <c r="AU6" s="116"/>
-      <c r="AV6" s="116"/>
-      <c r="AW6" s="116"/>
-      <c r="AX6" s="116"/>
-      <c r="AY6" s="116"/>
-      <c r="AZ6" s="116"/>
-      <c r="BA6" s="116"/>
-      <c r="BB6" s="116"/>
-      <c r="BC6" s="116"/>
-      <c r="BD6" s="116"/>
-      <c r="BE6" s="116"/>
-      <c r="BF6" s="116"/>
-      <c r="BG6" s="116"/>
-      <c r="BH6" s="116"/>
-      <c r="BI6" s="116"/>
-      <c r="BJ6" s="116"/>
-      <c r="BK6" s="116"/>
-      <c r="BL6" s="116"/>
-      <c r="BM6" s="116"/>
-      <c r="BN6" s="116"/>
-      <c r="BO6" s="116"/>
-      <c r="BP6" s="116"/>
-      <c r="BQ6" s="116"/>
-      <c r="BR6" s="116"/>
-      <c r="BS6" s="116"/>
-      <c r="BT6" s="116"/>
-      <c r="BU6" s="116"/>
-      <c r="BV6" s="116"/>
-      <c r="BW6" s="116"/>
-      <c r="BX6" s="116"/>
-      <c r="BY6" s="116"/>
-      <c r="BZ6" s="116"/>
-      <c r="CA6" s="116"/>
-      <c r="CB6" s="116"/>
-      <c r="CC6" s="116"/>
-      <c r="CD6" s="116"/>
-      <c r="CE6" s="116"/>
-      <c r="CF6" s="116"/>
-      <c r="CG6" s="116"/>
-      <c r="CH6" s="116"/>
-      <c r="CI6" s="116"/>
-      <c r="CJ6" s="116"/>
-      <c r="CK6" s="116"/>
-      <c r="CL6" s="116"/>
-      <c r="CM6" s="116"/>
-      <c r="CN6" s="116"/>
-      <c r="CO6" s="116"/>
-      <c r="CP6" s="116"/>
-      <c r="CQ6" s="116"/>
-      <c r="CR6" s="116"/>
-      <c r="CS6" s="116"/>
-      <c r="CT6" s="116"/>
-      <c r="CU6" s="116"/>
-      <c r="CV6" s="116"/>
-      <c r="CW6" s="116"/>
-      <c r="CX6" s="116"/>
-      <c r="CY6" s="116"/>
-      <c r="CZ6" s="116"/>
-      <c r="DA6" s="116"/>
-      <c r="DB6" s="116"/>
-      <c r="DC6" s="116"/>
-      <c r="DD6" s="116"/>
-      <c r="DE6" s="116"/>
-      <c r="DF6" s="116"/>
-      <c r="DG6" s="116"/>
-      <c r="DH6" s="116"/>
-      <c r="DI6" s="116"/>
-      <c r="DJ6" s="116"/>
-      <c r="DK6" s="116"/>
-      <c r="DL6" s="116"/>
-      <c r="DM6" s="116"/>
-      <c r="DN6" s="116"/>
-      <c r="DO6" s="116"/>
-      <c r="DP6" s="116"/>
-      <c r="DQ6" s="116"/>
-      <c r="DR6" s="116"/>
-      <c r="DS6" s="116"/>
-      <c r="DT6" s="116"/>
-      <c r="DU6" s="116"/>
-      <c r="DV6" s="116"/>
-      <c r="DW6" s="116"/>
-      <c r="DX6" s="116"/>
-      <c r="DY6" s="116"/>
-      <c r="DZ6" s="117"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="92"/>
+      <c r="L6" s="92"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="92"/>
+      <c r="O6" s="92"/>
+      <c r="P6" s="92"/>
+      <c r="Q6" s="92"/>
+      <c r="R6" s="92"/>
+      <c r="S6" s="92"/>
+      <c r="T6" s="92"/>
+      <c r="U6" s="92"/>
+      <c r="V6" s="92"/>
+      <c r="W6" s="92"/>
+      <c r="X6" s="92"/>
+      <c r="Y6" s="92"/>
+      <c r="Z6" s="92"/>
+      <c r="AA6" s="92"/>
+      <c r="AB6" s="92"/>
+      <c r="AC6" s="92"/>
+      <c r="AD6" s="92"/>
+      <c r="AE6" s="92"/>
+      <c r="AF6" s="92"/>
+      <c r="AG6" s="92"/>
+      <c r="AH6" s="92"/>
+      <c r="AI6" s="92"/>
+      <c r="AJ6" s="92"/>
+      <c r="AK6" s="92"/>
+      <c r="AL6" s="92"/>
+      <c r="AM6" s="92"/>
+      <c r="AN6" s="92"/>
+      <c r="AO6" s="92"/>
+      <c r="AP6" s="92"/>
+      <c r="AQ6" s="92"/>
+      <c r="AR6" s="92"/>
+      <c r="AS6" s="92"/>
+      <c r="AT6" s="92"/>
+      <c r="AU6" s="92"/>
+      <c r="AV6" s="92"/>
+      <c r="AW6" s="92"/>
+      <c r="AX6" s="92"/>
+      <c r="AY6" s="92"/>
+      <c r="AZ6" s="92"/>
+      <c r="BA6" s="92"/>
+      <c r="BB6" s="92"/>
+      <c r="BC6" s="92"/>
+      <c r="BD6" s="92"/>
+      <c r="BE6" s="92"/>
+      <c r="BF6" s="92"/>
+      <c r="BG6" s="92"/>
+      <c r="BH6" s="92"/>
+      <c r="BI6" s="92"/>
+      <c r="BJ6" s="92"/>
+      <c r="BK6" s="92"/>
+      <c r="BL6" s="92"/>
+      <c r="BM6" s="92"/>
+      <c r="BN6" s="92"/>
+      <c r="BO6" s="92"/>
+      <c r="BP6" s="92"/>
+      <c r="BQ6" s="92"/>
+      <c r="BR6" s="92"/>
+      <c r="BS6" s="92"/>
+      <c r="BT6" s="92"/>
+      <c r="BU6" s="92"/>
+      <c r="BV6" s="92"/>
+      <c r="BW6" s="92"/>
+      <c r="BX6" s="92"/>
+      <c r="BY6" s="92"/>
+      <c r="BZ6" s="92"/>
+      <c r="CA6" s="92"/>
+      <c r="CB6" s="92"/>
+      <c r="CC6" s="92"/>
+      <c r="CD6" s="92"/>
+      <c r="CE6" s="92"/>
+      <c r="CF6" s="92"/>
+      <c r="CG6" s="92"/>
+      <c r="CH6" s="92"/>
+      <c r="CI6" s="92"/>
+      <c r="CJ6" s="92"/>
+      <c r="CK6" s="92"/>
+      <c r="CL6" s="92"/>
+      <c r="CM6" s="92"/>
+      <c r="CN6" s="92"/>
+      <c r="CO6" s="92"/>
+      <c r="CP6" s="92"/>
+      <c r="CQ6" s="92"/>
+      <c r="CR6" s="92"/>
+      <c r="CS6" s="92"/>
+      <c r="CT6" s="92"/>
+      <c r="CU6" s="92"/>
+      <c r="CV6" s="92"/>
+      <c r="CW6" s="92"/>
+      <c r="CX6" s="92"/>
+      <c r="CY6" s="92"/>
+      <c r="CZ6" s="92"/>
+      <c r="DA6" s="92"/>
+      <c r="DB6" s="92"/>
+      <c r="DC6" s="92"/>
+      <c r="DD6" s="92"/>
+      <c r="DE6" s="92"/>
+      <c r="DF6" s="92"/>
+      <c r="DG6" s="92"/>
+      <c r="DH6" s="92"/>
+      <c r="DI6" s="92"/>
+      <c r="DJ6" s="92"/>
+      <c r="DK6" s="92"/>
+      <c r="DL6" s="92"/>
+      <c r="DM6" s="92"/>
+      <c r="DN6" s="92"/>
+      <c r="DO6" s="92"/>
+      <c r="DP6" s="92"/>
+      <c r="DQ6" s="92"/>
+      <c r="DR6" s="92"/>
+      <c r="DS6" s="92"/>
+      <c r="DT6" s="92"/>
+      <c r="DU6" s="92"/>
+      <c r="DV6" s="92"/>
+      <c r="DW6" s="92"/>
+      <c r="DX6" s="92"/>
+      <c r="DY6" s="92"/>
+      <c r="DZ6" s="93"/>
     </row>
     <row r="7" spans="1:130">
-      <c r="A7" s="87"/>
+      <c r="A7" s="113"/>
       <c r="B7" s="84">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -2804,7 +2813,7 @@
       <c r="DZ7" s="35"/>
     </row>
     <row r="8" spans="1:130">
-      <c r="A8" s="87"/>
+      <c r="A8" s="113"/>
       <c r="B8" s="84">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -2939,7 +2948,7 @@
       <c r="DZ8" s="38"/>
     </row>
     <row r="9" spans="1:130">
-      <c r="A9" s="87"/>
+      <c r="A9" s="113"/>
       <c r="B9" s="84">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -3009,7 +3018,7 @@
       <c r="BK9" s="20"/>
       <c r="BL9" s="21"/>
       <c r="BM9" s="24" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="BN9" s="21"/>
       <c r="BO9" s="21"/>
@@ -3066,7 +3075,7 @@
       <c r="DN9" s="22"/>
       <c r="DO9" s="37"/>
       <c r="DP9" s="36"/>
-      <c r="DQ9" s="119" t="s">
+      <c r="DQ9" s="94" t="s">
         <v>6</v>
       </c>
       <c r="DR9" s="36"/>
@@ -3080,7 +3089,7 @@
       <c r="DZ9" s="38"/>
     </row>
     <row r="10" spans="1:130">
-      <c r="A10" s="87"/>
+      <c r="A10" s="113"/>
       <c r="B10" s="84">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -3149,7 +3158,9 @@
       <c r="BJ10" s="19"/>
       <c r="BK10" s="20"/>
       <c r="BL10" s="21"/>
-      <c r="BM10" s="21"/>
+      <c r="BM10" s="24" t="s">
+        <v>4</v>
+      </c>
       <c r="BN10" s="21"/>
       <c r="BO10" s="21"/>
       <c r="BP10" s="21"/>
@@ -3205,7 +3216,7 @@
       <c r="DN10" s="22"/>
       <c r="DO10" s="37"/>
       <c r="DP10" s="36"/>
-      <c r="DQ10" s="119" t="s">
+      <c r="DQ10" s="94" t="s">
         <v>5</v>
       </c>
       <c r="DR10" s="36"/>
@@ -3219,7 +3230,7 @@
       <c r="DZ10" s="38"/>
     </row>
     <row r="11" spans="1:130">
-      <c r="A11" s="87"/>
+      <c r="A11" s="113"/>
       <c r="B11" s="84">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -3354,7 +3365,7 @@
       <c r="DZ11" s="38"/>
     </row>
     <row r="12" spans="1:130">
-      <c r="A12" s="87"/>
+      <c r="A12" s="113"/>
       <c r="B12" s="84">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -3489,7 +3500,7 @@
       <c r="DZ12" s="38"/>
     </row>
     <row r="13" spans="1:130">
-      <c r="A13" s="87"/>
+      <c r="A13" s="113"/>
       <c r="B13" s="84">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -3624,7 +3635,7 @@
       <c r="DZ13" s="38"/>
     </row>
     <row r="14" spans="1:130">
-      <c r="A14" s="87"/>
+      <c r="A14" s="113"/>
       <c r="B14" s="84">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -3759,7 +3770,7 @@
       <c r="DZ14" s="38"/>
     </row>
     <row r="15" spans="1:130">
-      <c r="A15" s="87"/>
+      <c r="A15" s="113"/>
       <c r="B15" s="84">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -3894,7 +3905,7 @@
       <c r="DZ15" s="38"/>
     </row>
     <row r="16" spans="1:130">
-      <c r="A16" s="87"/>
+      <c r="A16" s="113"/>
       <c r="B16" s="84">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -4029,7 +4040,7 @@
       <c r="DZ16" s="38"/>
     </row>
     <row r="17" spans="1:130">
-      <c r="A17" s="87"/>
+      <c r="A17" s="113"/>
       <c r="B17" s="84">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -4164,7 +4175,7 @@
       <c r="DZ17" s="38"/>
     </row>
     <row r="18" spans="1:130" ht="17" thickBot="1">
-      <c r="A18" s="88"/>
+      <c r="A18" s="114"/>
       <c r="B18" s="85">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -4299,7 +4310,7 @@
       <c r="DZ18" s="38"/>
     </row>
     <row r="19" spans="1:130">
-      <c r="A19" s="89" t="s">
+      <c r="A19" s="115" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="83">
@@ -4436,7 +4447,7 @@
       <c r="DZ19" s="38"/>
     </row>
     <row r="20" spans="1:130">
-      <c r="A20" s="90"/>
+      <c r="A20" s="116"/>
       <c r="B20" s="84">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -4571,7 +4582,7 @@
       <c r="DZ20" s="38"/>
     </row>
     <row r="21" spans="1:130">
-      <c r="A21" s="90"/>
+      <c r="A21" s="116"/>
       <c r="B21" s="84">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -4706,7 +4717,7 @@
       <c r="DZ21" s="38"/>
     </row>
     <row r="22" spans="1:130">
-      <c r="A22" s="90"/>
+      <c r="A22" s="116"/>
       <c r="B22" s="84">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -4841,7 +4852,7 @@
       <c r="DZ22" s="38"/>
     </row>
     <row r="23" spans="1:130">
-      <c r="A23" s="90"/>
+      <c r="A23" s="116"/>
       <c r="B23" s="84">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -4976,7 +4987,7 @@
       <c r="DZ23" s="38"/>
     </row>
     <row r="24" spans="1:130">
-      <c r="A24" s="90"/>
+      <c r="A24" s="116"/>
       <c r="B24" s="84">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -5111,7 +5122,7 @@
       <c r="DZ24" s="38"/>
     </row>
     <row r="25" spans="1:130">
-      <c r="A25" s="90"/>
+      <c r="A25" s="116"/>
       <c r="B25" s="84">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -5246,7 +5257,7 @@
       <c r="DZ25" s="38"/>
     </row>
     <row r="26" spans="1:130">
-      <c r="A26" s="90"/>
+      <c r="A26" s="116"/>
       <c r="B26" s="84">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -5381,7 +5392,7 @@
       <c r="DZ26" s="38"/>
     </row>
     <row r="27" spans="1:130">
-      <c r="A27" s="90"/>
+      <c r="A27" s="116"/>
       <c r="B27" s="84">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -5516,7 +5527,7 @@
       <c r="DZ27" s="38"/>
     </row>
     <row r="28" spans="1:130">
-      <c r="A28" s="90"/>
+      <c r="A28" s="116"/>
       <c r="B28" s="84">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -5651,7 +5662,7 @@
       <c r="DZ28" s="38"/>
     </row>
     <row r="29" spans="1:130">
-      <c r="A29" s="90"/>
+      <c r="A29" s="116"/>
       <c r="B29" s="84">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -5786,7 +5797,7 @@
       <c r="DZ29" s="38"/>
     </row>
     <row r="30" spans="1:130">
-      <c r="A30" s="90"/>
+      <c r="A30" s="116"/>
       <c r="B30" s="84">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -5921,7 +5932,7 @@
       <c r="DZ30" s="38"/>
     </row>
     <row r="31" spans="1:130">
-      <c r="A31" s="90"/>
+      <c r="A31" s="116"/>
       <c r="B31" s="84">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -6056,7 +6067,7 @@
       <c r="DZ31" s="38"/>
     </row>
     <row r="32" spans="1:130">
-      <c r="A32" s="90"/>
+      <c r="A32" s="116"/>
       <c r="B32" s="84">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -6191,7 +6202,7 @@
       <c r="DZ32" s="38"/>
     </row>
     <row r="33" spans="1:132">
-      <c r="A33" s="90"/>
+      <c r="A33" s="116"/>
       <c r="B33" s="84">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -6326,7 +6337,7 @@
       <c r="DZ33" s="38"/>
     </row>
     <row r="34" spans="1:132" ht="17" customHeight="1" thickBot="1">
-      <c r="A34" s="91"/>
+      <c r="A34" s="117"/>
       <c r="B34" s="85">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -6459,12 +6470,12 @@
       <c r="DX34" s="37"/>
       <c r="DY34" s="37"/>
       <c r="DZ34" s="38"/>
-      <c r="EB34" s="118" t="s">
+      <c r="EB34" s="96" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:132" ht="17" customHeight="1">
-      <c r="A35" s="86" t="s">
+      <c r="A35" s="112" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="83">
@@ -6599,10 +6610,10 @@
       <c r="DX35" s="37"/>
       <c r="DY35" s="37"/>
       <c r="DZ35" s="38"/>
-      <c r="EB35" s="118"/>
+      <c r="EB35" s="96"/>
     </row>
     <row r="36" spans="1:132">
-      <c r="A36" s="87"/>
+      <c r="A36" s="113"/>
       <c r="B36" s="84">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -6737,7 +6748,7 @@
       <c r="DZ36" s="38"/>
     </row>
     <row r="37" spans="1:132">
-      <c r="A37" s="87"/>
+      <c r="A37" s="113"/>
       <c r="B37" s="84">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -6872,7 +6883,7 @@
       <c r="DZ37" s="38"/>
     </row>
     <row r="38" spans="1:132">
-      <c r="A38" s="87"/>
+      <c r="A38" s="113"/>
       <c r="B38" s="84">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -7007,7 +7018,7 @@
       <c r="DZ38" s="38"/>
     </row>
     <row r="39" spans="1:132">
-      <c r="A39" s="87"/>
+      <c r="A39" s="113"/>
       <c r="B39" s="84">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -7142,7 +7153,7 @@
       <c r="DZ39" s="38"/>
     </row>
     <row r="40" spans="1:132">
-      <c r="A40" s="87"/>
+      <c r="A40" s="113"/>
       <c r="B40" s="84">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -7277,7 +7288,7 @@
       <c r="DZ40" s="38"/>
     </row>
     <row r="41" spans="1:132">
-      <c r="A41" s="87"/>
+      <c r="A41" s="113"/>
       <c r="B41" s="84">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -7412,7 +7423,7 @@
       <c r="DZ41" s="38"/>
     </row>
     <row r="42" spans="1:132">
-      <c r="A42" s="87"/>
+      <c r="A42" s="113"/>
       <c r="B42" s="84">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -7547,7 +7558,7 @@
       <c r="DZ42" s="38"/>
     </row>
     <row r="43" spans="1:132">
-      <c r="A43" s="87"/>
+      <c r="A43" s="113"/>
       <c r="B43" s="84">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -7682,7 +7693,7 @@
       <c r="DZ43" s="38"/>
     </row>
     <row r="44" spans="1:132">
-      <c r="A44" s="87"/>
+      <c r="A44" s="113"/>
       <c r="B44" s="84">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -7817,7 +7828,7 @@
       <c r="DZ44" s="38"/>
     </row>
     <row r="45" spans="1:132">
-      <c r="A45" s="87"/>
+      <c r="A45" s="113"/>
       <c r="B45" s="84">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -7952,7 +7963,7 @@
       <c r="DZ45" s="38"/>
     </row>
     <row r="46" spans="1:132">
-      <c r="A46" s="87"/>
+      <c r="A46" s="113"/>
       <c r="B46" s="84">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -8087,7 +8098,7 @@
       <c r="DZ46" s="38"/>
     </row>
     <row r="47" spans="1:132">
-      <c r="A47" s="87"/>
+      <c r="A47" s="113"/>
       <c r="B47" s="84">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -8222,7 +8233,7 @@
       <c r="DZ47" s="38"/>
     </row>
     <row r="48" spans="1:132">
-      <c r="A48" s="87"/>
+      <c r="A48" s="113"/>
       <c r="B48" s="84">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -8357,7 +8368,7 @@
       <c r="DZ48" s="38"/>
     </row>
     <row r="49" spans="1:130">
-      <c r="A49" s="87"/>
+      <c r="A49" s="113"/>
       <c r="B49" s="84">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -8492,7 +8503,7 @@
       <c r="DZ49" s="38"/>
     </row>
     <row r="50" spans="1:130" ht="17" thickBot="1">
-      <c r="A50" s="88"/>
+      <c r="A50" s="114"/>
       <c r="B50" s="85">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -8627,7 +8638,7 @@
       <c r="DZ50" s="38"/>
     </row>
     <row r="51" spans="1:130">
-      <c r="A51" s="89" t="s">
+      <c r="A51" s="115" t="s">
         <v>36</v>
       </c>
       <c r="B51" s="83">
@@ -8764,7 +8775,7 @@
       <c r="DZ51" s="38"/>
     </row>
     <row r="52" spans="1:130">
-      <c r="A52" s="90"/>
+      <c r="A52" s="116"/>
       <c r="B52" s="84">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -8899,7 +8910,7 @@
       <c r="DZ52" s="38"/>
     </row>
     <row r="53" spans="1:130">
-      <c r="A53" s="90"/>
+      <c r="A53" s="116"/>
       <c r="B53" s="84">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -9034,7 +9045,7 @@
       <c r="DZ53" s="38"/>
     </row>
     <row r="54" spans="1:130">
-      <c r="A54" s="90"/>
+      <c r="A54" s="116"/>
       <c r="B54" s="84">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -9169,7 +9180,7 @@
       <c r="DZ54" s="38"/>
     </row>
     <row r="55" spans="1:130">
-      <c r="A55" s="90"/>
+      <c r="A55" s="116"/>
       <c r="B55" s="84">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -9304,7 +9315,7 @@
       <c r="DZ55" s="38"/>
     </row>
     <row r="56" spans="1:130">
-      <c r="A56" s="90"/>
+      <c r="A56" s="116"/>
       <c r="B56" s="84">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -9439,7 +9450,7 @@
       <c r="DZ56" s="38"/>
     </row>
     <row r="57" spans="1:130">
-      <c r="A57" s="90"/>
+      <c r="A57" s="116"/>
       <c r="B57" s="84">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -9574,7 +9585,7 @@
       <c r="DZ57" s="38"/>
     </row>
     <row r="58" spans="1:130">
-      <c r="A58" s="90"/>
+      <c r="A58" s="116"/>
       <c r="B58" s="84">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -9709,7 +9720,7 @@
       <c r="DZ58" s="38"/>
     </row>
     <row r="59" spans="1:130">
-      <c r="A59" s="90"/>
+      <c r="A59" s="116"/>
       <c r="B59" s="84">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -9844,7 +9855,7 @@
       <c r="DZ59" s="38"/>
     </row>
     <row r="60" spans="1:130">
-      <c r="A60" s="90"/>
+      <c r="A60" s="116"/>
       <c r="B60" s="84">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -9979,7 +9990,7 @@
       <c r="DZ60" s="38"/>
     </row>
     <row r="61" spans="1:130">
-      <c r="A61" s="90"/>
+      <c r="A61" s="116"/>
       <c r="B61" s="84">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -10114,7 +10125,7 @@
       <c r="DZ61" s="38"/>
     </row>
     <row r="62" spans="1:130" ht="17" thickBot="1">
-      <c r="A62" s="90"/>
+      <c r="A62" s="116"/>
       <c r="B62" s="84">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -10249,7 +10260,7 @@
       <c r="DZ62" s="43"/>
     </row>
     <row r="63" spans="1:130">
-      <c r="A63" s="90"/>
+      <c r="A63" s="116"/>
       <c r="B63" s="84">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -10384,7 +10395,7 @@
       <c r="DZ63" s="32"/>
     </row>
     <row r="64" spans="1:130">
-      <c r="A64" s="90"/>
+      <c r="A64" s="116"/>
       <c r="B64" s="84">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -10519,7 +10530,7 @@
       <c r="DZ64" s="32"/>
     </row>
     <row r="65" spans="1:130">
-      <c r="A65" s="90"/>
+      <c r="A65" s="116"/>
       <c r="B65" s="84">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -10654,7 +10665,7 @@
       <c r="DZ65" s="32"/>
     </row>
     <row r="66" spans="1:130" ht="17" thickBot="1">
-      <c r="A66" s="91"/>
+      <c r="A66" s="117"/>
       <c r="B66" s="85">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -10791,10 +10802,10 @@
     <row r="70" spans="1:130" s="55" customFormat="1" ht="24">
       <c r="B70" s="54"/>
       <c r="AE70" s="56"/>
-      <c r="AF70" s="93">
+      <c r="AF70" s="118">
         <v>60</v>
       </c>
-      <c r="AG70" s="93"/>
+      <c r="AG70" s="118"/>
       <c r="AH70" s="56"/>
       <c r="AI70" s="56"/>
       <c r="AJ70" s="56"/>
@@ -10884,10 +10895,10 @@
       <c r="DO70" s="56"/>
       <c r="DR70" s="56"/>
       <c r="DS70" s="56"/>
-      <c r="DT70" s="93" t="s">
+      <c r="DT70" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="DU70" s="93"/>
+      <c r="DU70" s="118"/>
       <c r="DV70" s="56"/>
       <c r="DW70" s="56"/>
       <c r="DX70" s="56"/>
@@ -11121,62 +11132,62 @@
       <c r="DZ72" s="51"/>
     </row>
     <row r="73" spans="1:130" ht="20">
-      <c r="C73" s="96" t="s">
+      <c r="C73" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="D73" s="96"/>
-      <c r="E73" s="96" t="s">
+      <c r="D73" s="104"/>
+      <c r="E73" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="F73" s="96"/>
-      <c r="G73" s="96"/>
-      <c r="H73" s="96" t="s">
+      <c r="F73" s="104"/>
+      <c r="G73" s="104"/>
+      <c r="H73" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="I73" s="96"/>
-      <c r="J73" s="96"/>
-      <c r="K73" s="96"/>
-      <c r="L73" s="96" t="s">
+      <c r="I73" s="104"/>
+      <c r="J73" s="104"/>
+      <c r="K73" s="104"/>
+      <c r="L73" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="M73" s="96"/>
-      <c r="N73" s="96"/>
+      <c r="M73" s="104"/>
+      <c r="N73" s="104"/>
       <c r="O73" s="46"/>
-      <c r="P73" s="96" t="s">
+      <c r="P73" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="Q73" s="96"/>
-      <c r="R73" s="96"/>
-      <c r="S73" s="96"/>
-      <c r="T73" s="96"/>
+      <c r="Q73" s="104"/>
+      <c r="R73" s="104"/>
+      <c r="S73" s="104"/>
+      <c r="T73" s="104"/>
       <c r="U73" s="47" t="s">
         <v>13</v>
       </c>
       <c r="V73" s="47"/>
       <c r="W73" s="47"/>
       <c r="X73" s="47"/>
-      <c r="AN73" s="96" t="s">
+      <c r="AN73" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="AO73" s="96"/>
-      <c r="AP73" s="96" t="s">
+      <c r="AO73" s="104"/>
+      <c r="AP73" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="AQ73" s="96"/>
-      <c r="AR73" s="96"/>
-      <c r="AS73" s="96" t="s">
+      <c r="AQ73" s="104"/>
+      <c r="AR73" s="104"/>
+      <c r="AS73" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="AT73" s="96"/>
-      <c r="AU73" s="96"/>
-      <c r="AV73" s="96"/>
-      <c r="AW73" s="96" t="s">
+      <c r="AT73" s="104"/>
+      <c r="AU73" s="104"/>
+      <c r="AV73" s="104"/>
+      <c r="AW73" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="AX73" s="96"/>
-      <c r="AY73" s="96"/>
-      <c r="AZ73" s="96"/>
-      <c r="BA73" s="96"/>
+      <c r="AX73" s="104"/>
+      <c r="AY73" s="104"/>
+      <c r="AZ73" s="104"/>
+      <c r="BA73" s="104"/>
       <c r="BB73" s="58" t="s">
         <v>25</v>
       </c>
@@ -11184,13 +11195,13 @@
       <c r="BD73" s="58"/>
       <c r="BE73" s="58"/>
       <c r="BF73" s="47"/>
-      <c r="BG73" s="96" t="s">
+      <c r="BG73" s="104" t="s">
         <v>28</v>
       </c>
-      <c r="BH73" s="96"/>
-      <c r="BI73" s="96"/>
-      <c r="BJ73" s="96"/>
-      <c r="BK73" s="96"/>
+      <c r="BH73" s="104"/>
+      <c r="BI73" s="104"/>
+      <c r="BJ73" s="104"/>
+      <c r="BK73" s="104"/>
       <c r="BL73" s="58" t="s">
         <v>26</v>
       </c>
@@ -11204,40 +11215,40 @@
       <c r="BT73" s="46"/>
     </row>
     <row r="74" spans="1:130" ht="20">
-      <c r="C74" s="94">
+      <c r="C74" s="111">
         <v>5</v>
       </c>
-      <c r="D74" s="94"/>
-      <c r="E74" s="94">
+      <c r="D74" s="111"/>
+      <c r="E74" s="111">
         <v>3</v>
       </c>
-      <c r="F74" s="94"/>
-      <c r="G74" s="94"/>
-      <c r="H74" s="94" t="s">
+      <c r="F74" s="111"/>
+      <c r="G74" s="111"/>
+      <c r="H74" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="I74" s="94"/>
-      <c r="J74" s="94"/>
-      <c r="K74" s="94"/>
-      <c r="L74" s="95" t="s">
+      <c r="I74" s="111"/>
+      <c r="J74" s="111"/>
+      <c r="K74" s="111"/>
+      <c r="L74" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="M74" s="95"/>
-      <c r="N74" s="95"/>
-      <c r="P74" s="94">
+      <c r="M74" s="119"/>
+      <c r="N74" s="119"/>
+      <c r="P74" s="111">
         <f t="shared" ref="P74:P88" si="2">61*60+60*(68-C74)+(68-C74)*C74</f>
         <v>7755</v>
       </c>
-      <c r="Q74" s="94"/>
-      <c r="R74" s="94"/>
-      <c r="S74" s="94"/>
-      <c r="T74" s="94"/>
-      <c r="U74" s="97">
+      <c r="Q74" s="111"/>
+      <c r="R74" s="111"/>
+      <c r="S74" s="111"/>
+      <c r="T74" s="111"/>
+      <c r="U74" s="107">
         <f t="shared" ref="U74:U88" si="3">C74*FLOOR(IF(E74=3,15,16)/E74,1)^2*10</f>
         <v>1250</v>
       </c>
-      <c r="V74" s="97"/>
-      <c r="W74" s="97"/>
+      <c r="V74" s="107"/>
+      <c r="W74" s="107"/>
       <c r="X74" s="48"/>
       <c r="Z74" s="52" t="s">
         <v>16</v>
@@ -11245,58 +11256,58 @@
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
       <c r="AC74" s="1"/>
-      <c r="AN74" s="101">
+      <c r="AN74" s="97">
         <v>1</v>
       </c>
-      <c r="AO74" s="101"/>
-      <c r="AP74" s="101">
+      <c r="AO74" s="97"/>
+      <c r="AP74" s="97">
         <v>1</v>
       </c>
-      <c r="AQ74" s="101"/>
-      <c r="AR74" s="101"/>
-      <c r="AS74" s="101">
+      <c r="AQ74" s="97"/>
+      <c r="AR74" s="97"/>
+      <c r="AS74" s="97">
         <v>60</v>
       </c>
-      <c r="AT74" s="101"/>
-      <c r="AU74" s="101"/>
-      <c r="AV74" s="101"/>
-      <c r="AW74" s="102">
+      <c r="AT74" s="97"/>
+      <c r="AU74" s="97"/>
+      <c r="AV74" s="97"/>
+      <c r="AW74" s="99">
         <v>28</v>
       </c>
-      <c r="AX74" s="102"/>
+      <c r="AX74" s="99"/>
       <c r="AY74" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="AZ74" s="102">
+      <c r="AZ74" s="99">
         <v>28</v>
       </c>
-      <c r="BA74" s="102"/>
-      <c r="BB74" s="101">
+      <c r="BA74" s="99"/>
+      <c r="BB74" s="97">
         <f>AP74*AW74*AZ74</f>
         <v>784</v>
       </c>
-      <c r="BC74" s="101"/>
-      <c r="BD74" s="101"/>
-      <c r="BE74" s="101"/>
+      <c r="BC74" s="97"/>
+      <c r="BD74" s="97"/>
+      <c r="BE74" s="97"/>
       <c r="BF74" s="61"/>
-      <c r="BG74" s="102">
+      <c r="BG74" s="99">
         <v>30</v>
       </c>
-      <c r="BH74" s="102"/>
+      <c r="BH74" s="99"/>
       <c r="BI74" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="BJ74" s="102">
+      <c r="BJ74" s="99">
         <v>30</v>
       </c>
-      <c r="BK74" s="102"/>
-      <c r="BL74" s="101">
+      <c r="BK74" s="99"/>
+      <c r="BL74" s="97">
         <f>AS74*BG74*BJ74</f>
         <v>54000</v>
       </c>
-      <c r="BM74" s="101"/>
-      <c r="BN74" s="101"/>
-      <c r="BO74" s="101"/>
+      <c r="BM74" s="97"/>
+      <c r="BN74" s="97"/>
+      <c r="BO74" s="97"/>
       <c r="BR74" s="63" t="s">
         <v>0</v>
       </c>
@@ -11305,370 +11316,370 @@
       <c r="BU74" s="63"/>
     </row>
     <row r="75" spans="1:130" ht="20">
-      <c r="C75" s="97">
+      <c r="C75" s="107">
         <v>10</v>
       </c>
-      <c r="D75" s="97"/>
-      <c r="E75" s="97">
+      <c r="D75" s="107"/>
+      <c r="E75" s="107">
         <v>3</v>
       </c>
-      <c r="F75" s="97"/>
-      <c r="G75" s="97"/>
-      <c r="H75" s="92" t="s">
+      <c r="F75" s="107"/>
+      <c r="G75" s="107"/>
+      <c r="H75" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="I75" s="92"/>
-      <c r="J75" s="92"/>
-      <c r="K75" s="92"/>
-      <c r="L75" s="98" t="s">
+      <c r="I75" s="108"/>
+      <c r="J75" s="108"/>
+      <c r="K75" s="108"/>
+      <c r="L75" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="M75" s="98"/>
-      <c r="N75" s="98"/>
-      <c r="P75" s="97">
+      <c r="M75" s="106"/>
+      <c r="N75" s="106"/>
+      <c r="P75" s="107">
         <f t="shared" si="2"/>
         <v>7720</v>
       </c>
-      <c r="Q75" s="97"/>
-      <c r="R75" s="97"/>
-      <c r="S75" s="97"/>
-      <c r="T75" s="97"/>
-      <c r="U75" s="97">
+      <c r="Q75" s="107"/>
+      <c r="R75" s="107"/>
+      <c r="S75" s="107"/>
+      <c r="T75" s="107"/>
+      <c r="U75" s="107">
         <f t="shared" si="3"/>
         <v>2500</v>
       </c>
-      <c r="V75" s="97"/>
-      <c r="W75" s="97"/>
+      <c r="V75" s="107"/>
+      <c r="W75" s="107"/>
       <c r="X75" s="48"/>
-      <c r="AN75" s="97">
+      <c r="AN75" s="107">
         <v>2</v>
       </c>
-      <c r="AO75" s="97"/>
-      <c r="AP75" s="97">
+      <c r="AO75" s="107"/>
+      <c r="AP75" s="107">
         <v>60</v>
       </c>
-      <c r="AQ75" s="97"/>
-      <c r="AR75" s="97"/>
-      <c r="AS75" s="92">
+      <c r="AQ75" s="107"/>
+      <c r="AR75" s="107"/>
+      <c r="AS75" s="108">
         <v>60</v>
       </c>
-      <c r="AT75" s="92"/>
-      <c r="AU75" s="92"/>
-      <c r="AV75" s="92"/>
-      <c r="AW75" s="103">
+      <c r="AT75" s="108"/>
+      <c r="AU75" s="108"/>
+      <c r="AV75" s="108"/>
+      <c r="AW75" s="105">
         <v>30</v>
       </c>
-      <c r="AX75" s="103"/>
+      <c r="AX75" s="105"/>
       <c r="AY75" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="AZ75" s="103">
+      <c r="AZ75" s="105">
         <v>30</v>
       </c>
-      <c r="BA75" s="103"/>
-      <c r="BB75" s="101">
+      <c r="BA75" s="105"/>
+      <c r="BB75" s="97">
         <f>AP75*AW75*AZ75</f>
         <v>54000</v>
       </c>
-      <c r="BC75" s="101"/>
-      <c r="BD75" s="101"/>
-      <c r="BE75" s="101"/>
+      <c r="BC75" s="97"/>
+      <c r="BD75" s="97"/>
+      <c r="BE75" s="97"/>
       <c r="BF75" s="61"/>
-      <c r="BG75" s="102">
+      <c r="BG75" s="99">
         <v>15</v>
       </c>
-      <c r="BH75" s="102"/>
+      <c r="BH75" s="99"/>
       <c r="BI75" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="BJ75" s="102">
+      <c r="BJ75" s="99">
         <v>15</v>
       </c>
-      <c r="BK75" s="102"/>
-      <c r="BL75" s="101">
+      <c r="BK75" s="99"/>
+      <c r="BL75" s="97">
         <f>AS75*BG75*BJ75</f>
         <v>13500</v>
       </c>
-      <c r="BM75" s="101"/>
-      <c r="BN75" s="101"/>
-      <c r="BO75" s="101"/>
+      <c r="BM75" s="97"/>
+      <c r="BN75" s="97"/>
+      <c r="BO75" s="97"/>
       <c r="BR75" s="63" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:130" ht="20">
-      <c r="C76" s="97">
+      <c r="C76" s="107">
         <v>10</v>
       </c>
-      <c r="D76" s="97"/>
-      <c r="E76" s="97">
+      <c r="D76" s="107"/>
+      <c r="E76" s="107">
         <v>3</v>
       </c>
-      <c r="F76" s="97"/>
-      <c r="G76" s="97"/>
-      <c r="H76" s="92" t="s">
+      <c r="F76" s="107"/>
+      <c r="G76" s="107"/>
+      <c r="H76" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="I76" s="92"/>
-      <c r="J76" s="92"/>
-      <c r="K76" s="92"/>
-      <c r="L76" s="98" t="s">
+      <c r="I76" s="108"/>
+      <c r="J76" s="108"/>
+      <c r="K76" s="108"/>
+      <c r="L76" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="M76" s="98"/>
-      <c r="N76" s="98"/>
-      <c r="P76" s="97">
+      <c r="M76" s="106"/>
+      <c r="N76" s="106"/>
+      <c r="P76" s="107">
         <f t="shared" si="2"/>
         <v>7720</v>
       </c>
-      <c r="Q76" s="97"/>
-      <c r="R76" s="97"/>
-      <c r="S76" s="97"/>
-      <c r="T76" s="97"/>
-      <c r="U76" s="97">
+      <c r="Q76" s="107"/>
+      <c r="R76" s="107"/>
+      <c r="S76" s="107"/>
+      <c r="T76" s="107"/>
+      <c r="U76" s="107">
         <f t="shared" si="3"/>
         <v>2500</v>
       </c>
-      <c r="V76" s="97"/>
-      <c r="W76" s="97"/>
+      <c r="V76" s="107"/>
+      <c r="W76" s="107"/>
       <c r="X76" s="48"/>
-      <c r="AN76" s="97">
+      <c r="AN76" s="107">
         <v>3</v>
       </c>
-      <c r="AO76" s="97"/>
-      <c r="AP76" s="97">
+      <c r="AO76" s="107"/>
+      <c r="AP76" s="107">
         <v>60</v>
       </c>
-      <c r="AQ76" s="97"/>
-      <c r="AR76" s="97"/>
-      <c r="AS76" s="92">
+      <c r="AQ76" s="107"/>
+      <c r="AR76" s="107"/>
+      <c r="AS76" s="108">
         <v>56</v>
       </c>
-      <c r="AT76" s="92"/>
-      <c r="AU76" s="92"/>
-      <c r="AV76" s="92"/>
-      <c r="AW76" s="103">
+      <c r="AT76" s="108"/>
+      <c r="AU76" s="108"/>
+      <c r="AV76" s="108"/>
+      <c r="AW76" s="105">
         <v>15</v>
       </c>
-      <c r="AX76" s="103"/>
+      <c r="AX76" s="105"/>
       <c r="AY76" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="AZ76" s="103">
+      <c r="AZ76" s="105">
         <v>15</v>
       </c>
-      <c r="BA76" s="103"/>
-      <c r="BB76" s="101">
+      <c r="BA76" s="105"/>
+      <c r="BB76" s="97">
         <f>AP76*AW76*AZ76</f>
         <v>13500</v>
       </c>
-      <c r="BC76" s="101"/>
-      <c r="BD76" s="101"/>
-      <c r="BE76" s="101"/>
+      <c r="BC76" s="97"/>
+      <c r="BD76" s="97"/>
+      <c r="BE76" s="97"/>
       <c r="BF76" s="61"/>
-      <c r="BG76" s="102">
+      <c r="BG76" s="99">
         <v>15</v>
       </c>
-      <c r="BH76" s="102"/>
+      <c r="BH76" s="99"/>
       <c r="BI76" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="BJ76" s="102">
+      <c r="BJ76" s="99">
         <v>15</v>
       </c>
-      <c r="BK76" s="102"/>
-      <c r="BL76" s="101">
+      <c r="BK76" s="99"/>
+      <c r="BL76" s="97">
         <f>AS76*BG76*BJ76</f>
         <v>12600</v>
       </c>
-      <c r="BM76" s="101"/>
-      <c r="BN76" s="101"/>
-      <c r="BO76" s="101"/>
+      <c r="BM76" s="97"/>
+      <c r="BN76" s="97"/>
+      <c r="BO76" s="97"/>
       <c r="BR76" s="63" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:130" ht="20">
-      <c r="C77" s="97">
+      <c r="C77" s="107">
         <v>10</v>
       </c>
-      <c r="D77" s="97"/>
-      <c r="E77" s="97">
+      <c r="D77" s="107"/>
+      <c r="E77" s="107">
         <v>5</v>
       </c>
-      <c r="F77" s="97"/>
-      <c r="G77" s="97"/>
-      <c r="H77" s="92" t="s">
+      <c r="F77" s="107"/>
+      <c r="G77" s="107"/>
+      <c r="H77" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="I77" s="92"/>
-      <c r="J77" s="92"/>
-      <c r="K77" s="92"/>
-      <c r="L77" s="98">
+      <c r="I77" s="108"/>
+      <c r="J77" s="108"/>
+      <c r="K77" s="108"/>
+      <c r="L77" s="106">
         <v>93.2</v>
       </c>
-      <c r="M77" s="98"/>
-      <c r="N77" s="98"/>
-      <c r="P77" s="97">
+      <c r="M77" s="106"/>
+      <c r="N77" s="106"/>
+      <c r="P77" s="107">
         <f t="shared" si="2"/>
         <v>7720</v>
       </c>
-      <c r="Q77" s="97"/>
-      <c r="R77" s="97"/>
-      <c r="S77" s="97"/>
-      <c r="T77" s="97"/>
-      <c r="U77" s="97">
+      <c r="Q77" s="107"/>
+      <c r="R77" s="107"/>
+      <c r="S77" s="107"/>
+      <c r="T77" s="107"/>
+      <c r="U77" s="107">
         <f t="shared" si="3"/>
         <v>900</v>
       </c>
-      <c r="V77" s="97"/>
-      <c r="W77" s="97"/>
+      <c r="V77" s="107"/>
+      <c r="W77" s="107"/>
       <c r="X77" s="48"/>
-      <c r="AN77" s="97">
+      <c r="AN77" s="107">
         <v>4</v>
       </c>
-      <c r="AO77" s="97"/>
-      <c r="AP77" s="97">
+      <c r="AO77" s="107"/>
+      <c r="AP77" s="107">
         <v>56</v>
       </c>
-      <c r="AQ77" s="97"/>
-      <c r="AR77" s="97"/>
-      <c r="AS77" s="92">
+      <c r="AQ77" s="107"/>
+      <c r="AR77" s="107"/>
+      <c r="AS77" s="108">
         <v>12</v>
       </c>
-      <c r="AT77" s="92"/>
-      <c r="AU77" s="92"/>
-      <c r="AV77" s="92"/>
-      <c r="AW77" s="103">
+      <c r="AT77" s="108"/>
+      <c r="AU77" s="108"/>
+      <c r="AV77" s="108"/>
+      <c r="AW77" s="105">
         <v>15</v>
       </c>
-      <c r="AX77" s="103"/>
+      <c r="AX77" s="105"/>
       <c r="AY77" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="AZ77" s="103">
+      <c r="AZ77" s="105">
         <v>15</v>
       </c>
-      <c r="BA77" s="103"/>
-      <c r="BB77" s="101">
+      <c r="BA77" s="105"/>
+      <c r="BB77" s="97">
         <f>AP77*AW77*AZ77</f>
         <v>12600</v>
       </c>
-      <c r="BC77" s="101"/>
-      <c r="BD77" s="101"/>
-      <c r="BE77" s="101"/>
+      <c r="BC77" s="97"/>
+      <c r="BD77" s="97"/>
+      <c r="BE77" s="97"/>
       <c r="BF77" s="61"/>
-      <c r="BG77" s="102">
+      <c r="BG77" s="99">
         <v>5</v>
       </c>
-      <c r="BH77" s="102"/>
+      <c r="BH77" s="99"/>
       <c r="BI77" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="BJ77" s="102">
+      <c r="BJ77" s="99">
         <v>5</v>
       </c>
-      <c r="BK77" s="102"/>
-      <c r="BL77" s="101">
+      <c r="BK77" s="99"/>
+      <c r="BL77" s="97">
         <f>AS77*BG77*BJ77</f>
         <v>300</v>
       </c>
-      <c r="BM77" s="101"/>
-      <c r="BN77" s="101"/>
-      <c r="BO77" s="101"/>
+      <c r="BM77" s="97"/>
+      <c r="BN77" s="97"/>
+      <c r="BO77" s="97"/>
       <c r="BR77" s="63" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:130" ht="20">
-      <c r="C78" s="97">
+      <c r="C78" s="107">
         <v>12</v>
       </c>
-      <c r="D78" s="97"/>
-      <c r="E78" s="97">
+      <c r="D78" s="107"/>
+      <c r="E78" s="107">
         <v>3</v>
       </c>
-      <c r="F78" s="97"/>
-      <c r="G78" s="97"/>
-      <c r="H78" s="97" t="s">
+      <c r="F78" s="107"/>
+      <c r="G78" s="107"/>
+      <c r="H78" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="I78" s="97"/>
-      <c r="J78" s="97"/>
-      <c r="K78" s="97"/>
-      <c r="L78" s="98">
+      <c r="I78" s="107"/>
+      <c r="J78" s="107"/>
+      <c r="K78" s="107"/>
+      <c r="L78" s="106">
         <v>93.13</v>
       </c>
-      <c r="M78" s="98"/>
-      <c r="N78" s="98"/>
+      <c r="M78" s="106"/>
+      <c r="N78" s="106"/>
       <c r="O78" s="59"/>
-      <c r="P78" s="97">
+      <c r="P78" s="107">
         <f t="shared" si="2"/>
         <v>7692</v>
       </c>
-      <c r="Q78" s="97"/>
-      <c r="R78" s="97"/>
-      <c r="S78" s="97"/>
-      <c r="T78" s="97"/>
-      <c r="U78" s="97">
+      <c r="Q78" s="107"/>
+      <c r="R78" s="107"/>
+      <c r="S78" s="107"/>
+      <c r="T78" s="107"/>
+      <c r="U78" s="107">
         <f t="shared" si="3"/>
         <v>3000</v>
       </c>
-      <c r="V78" s="97"/>
-      <c r="W78" s="97"/>
+      <c r="V78" s="107"/>
+      <c r="W78" s="107"/>
       <c r="X78" s="48"/>
-      <c r="AN78" s="107">
+      <c r="AN78" s="102">
         <v>5</v>
       </c>
-      <c r="AO78" s="107"/>
-      <c r="AP78" s="107">
+      <c r="AO78" s="102"/>
+      <c r="AP78" s="102">
         <v>12</v>
       </c>
-      <c r="AQ78" s="107"/>
-      <c r="AR78" s="107"/>
-      <c r="AS78" s="105">
+      <c r="AQ78" s="102"/>
+      <c r="AR78" s="102"/>
+      <c r="AS78" s="101">
         <v>10</v>
       </c>
-      <c r="AT78" s="105"/>
-      <c r="AU78" s="105"/>
-      <c r="AV78" s="105"/>
-      <c r="AW78" s="104">
+      <c r="AT78" s="101"/>
+      <c r="AU78" s="101"/>
+      <c r="AV78" s="101"/>
+      <c r="AW78" s="103">
         <v>5</v>
       </c>
-      <c r="AX78" s="104"/>
+      <c r="AX78" s="103"/>
       <c r="AY78" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AZ78" s="104">
+      <c r="AZ78" s="103">
         <v>5</v>
       </c>
-      <c r="BA78" s="104"/>
-      <c r="BB78" s="105">
+      <c r="BA78" s="103"/>
+      <c r="BB78" s="101">
         <f>AP78*AW78*AZ78</f>
         <v>300</v>
       </c>
-      <c r="BC78" s="105"/>
-      <c r="BD78" s="105"/>
-      <c r="BE78" s="105"/>
+      <c r="BC78" s="101"/>
+      <c r="BD78" s="101"/>
+      <c r="BE78" s="101"/>
       <c r="BF78" s="66"/>
-      <c r="BG78" s="106">
+      <c r="BG78" s="100">
         <v>1</v>
       </c>
-      <c r="BH78" s="106"/>
+      <c r="BH78" s="100"/>
       <c r="BI78" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="BJ78" s="106">
+      <c r="BJ78" s="100">
         <v>10</v>
       </c>
-      <c r="BK78" s="106"/>
-      <c r="BL78" s="105">
+      <c r="BK78" s="100"/>
+      <c r="BL78" s="101">
         <f>AS78*BG78*BJ78</f>
         <v>100</v>
       </c>
-      <c r="BM78" s="105"/>
-      <c r="BN78" s="105"/>
-      <c r="BO78" s="105"/>
+      <c r="BM78" s="101"/>
+      <c r="BN78" s="101"/>
+      <c r="BO78" s="101"/>
       <c r="BP78" s="68"/>
       <c r="BQ78" s="68"/>
       <c r="BR78" s="69" t="s">
@@ -11678,77 +11689,77 @@
       <c r="BT78" s="68"/>
     </row>
     <row r="79" spans="1:130" ht="21" thickBot="1">
-      <c r="C79" s="97">
+      <c r="C79" s="107">
         <v>12</v>
       </c>
-      <c r="D79" s="97"/>
-      <c r="E79" s="97">
+      <c r="D79" s="107"/>
+      <c r="E79" s="107">
         <v>5</v>
       </c>
-      <c r="F79" s="97"/>
-      <c r="G79" s="97"/>
-      <c r="H79" s="92" t="s">
+      <c r="F79" s="107"/>
+      <c r="G79" s="107"/>
+      <c r="H79" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="I79" s="92"/>
-      <c r="J79" s="92"/>
-      <c r="K79" s="92"/>
-      <c r="L79" s="98">
+      <c r="I79" s="108"/>
+      <c r="J79" s="108"/>
+      <c r="K79" s="108"/>
+      <c r="L79" s="106">
         <v>93.23</v>
       </c>
-      <c r="M79" s="98"/>
-      <c r="N79" s="98"/>
-      <c r="P79" s="97">
+      <c r="M79" s="106"/>
+      <c r="N79" s="106"/>
+      <c r="P79" s="107">
         <f t="shared" si="2"/>
         <v>7692</v>
       </c>
-      <c r="Q79" s="97"/>
-      <c r="R79" s="97"/>
-      <c r="S79" s="97"/>
-      <c r="T79" s="97"/>
-      <c r="U79" s="97">
+      <c r="Q79" s="107"/>
+      <c r="R79" s="107"/>
+      <c r="S79" s="107"/>
+      <c r="T79" s="107"/>
+      <c r="U79" s="107">
         <f t="shared" si="3"/>
         <v>1080</v>
       </c>
-      <c r="V79" s="97"/>
-      <c r="W79" s="97"/>
+      <c r="V79" s="107"/>
+      <c r="W79" s="107"/>
       <c r="X79" s="48"/>
     </row>
     <row r="80" spans="1:130" ht="20">
-      <c r="C80" s="97">
+      <c r="C80" s="107">
         <v>15</v>
       </c>
-      <c r="D80" s="97"/>
-      <c r="E80" s="97">
+      <c r="D80" s="107"/>
+      <c r="E80" s="107">
         <v>3</v>
       </c>
-      <c r="F80" s="97"/>
-      <c r="G80" s="97"/>
-      <c r="H80" s="92" t="s">
+      <c r="F80" s="107"/>
+      <c r="G80" s="107"/>
+      <c r="H80" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="I80" s="92"/>
-      <c r="J80" s="92"/>
-      <c r="K80" s="92"/>
-      <c r="L80" s="98">
+      <c r="I80" s="108"/>
+      <c r="J80" s="108"/>
+      <c r="K80" s="108"/>
+      <c r="L80" s="106">
         <v>92.83</v>
       </c>
-      <c r="M80" s="98"/>
-      <c r="N80" s="98"/>
-      <c r="P80" s="97">
+      <c r="M80" s="106"/>
+      <c r="N80" s="106"/>
+      <c r="P80" s="107">
         <f t="shared" si="2"/>
         <v>7635</v>
       </c>
-      <c r="Q80" s="97"/>
-      <c r="R80" s="97"/>
-      <c r="S80" s="97"/>
-      <c r="T80" s="97"/>
-      <c r="U80" s="97">
+      <c r="Q80" s="107"/>
+      <c r="R80" s="107"/>
+      <c r="S80" s="107"/>
+      <c r="T80" s="107"/>
+      <c r="U80" s="107">
         <f t="shared" si="3"/>
         <v>3750</v>
       </c>
-      <c r="V80" s="97"/>
-      <c r="W80" s="97"/>
+      <c r="V80" s="107"/>
+      <c r="W80" s="107"/>
       <c r="X80" s="48"/>
       <c r="AL80" s="1"/>
       <c r="AM80" s="71"/>
@@ -11788,41 +11799,41 @@
       <c r="BU80" s="73"/>
     </row>
     <row r="81" spans="3:73" ht="20">
-      <c r="C81" s="97">
+      <c r="C81" s="107">
         <v>15</v>
       </c>
-      <c r="D81" s="97"/>
-      <c r="E81" s="97">
+      <c r="D81" s="107"/>
+      <c r="E81" s="107">
         <v>3</v>
       </c>
-      <c r="F81" s="97"/>
-      <c r="G81" s="97"/>
-      <c r="H81" s="97" t="s">
+      <c r="F81" s="107"/>
+      <c r="G81" s="107"/>
+      <c r="H81" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="I81" s="97"/>
-      <c r="J81" s="97"/>
-      <c r="K81" s="97"/>
-      <c r="L81" s="98">
+      <c r="I81" s="107"/>
+      <c r="J81" s="107"/>
+      <c r="K81" s="107"/>
+      <c r="L81" s="106">
         <v>93.45</v>
       </c>
-      <c r="M81" s="98"/>
-      <c r="N81" s="98"/>
+      <c r="M81" s="106"/>
+      <c r="N81" s="106"/>
       <c r="O81" s="59"/>
-      <c r="P81" s="97">
+      <c r="P81" s="107">
         <f t="shared" si="2"/>
         <v>7635</v>
       </c>
-      <c r="Q81" s="97"/>
-      <c r="R81" s="97"/>
-      <c r="S81" s="97"/>
-      <c r="T81" s="97"/>
-      <c r="U81" s="97">
+      <c r="Q81" s="107"/>
+      <c r="R81" s="107"/>
+      <c r="S81" s="107"/>
+      <c r="T81" s="107"/>
+      <c r="U81" s="107">
         <f t="shared" si="3"/>
         <v>3750</v>
       </c>
-      <c r="V81" s="97"/>
-      <c r="W81" s="97"/>
+      <c r="V81" s="107"/>
+      <c r="W81" s="107"/>
       <c r="X81" s="48"/>
       <c r="AL81" s="1"/>
       <c r="AM81" s="74"/>
@@ -11864,40 +11875,40 @@
       <c r="BU81" s="76"/>
     </row>
     <row r="82" spans="3:73" ht="20">
-      <c r="C82" s="97">
+      <c r="C82" s="107">
         <v>15</v>
       </c>
-      <c r="D82" s="97"/>
-      <c r="E82" s="97">
+      <c r="D82" s="107"/>
+      <c r="E82" s="107">
         <v>5</v>
       </c>
-      <c r="F82" s="97"/>
-      <c r="G82" s="97"/>
-      <c r="H82" s="92" t="s">
+      <c r="F82" s="107"/>
+      <c r="G82" s="107"/>
+      <c r="H82" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="I82" s="92"/>
-      <c r="J82" s="92"/>
-      <c r="K82" s="92"/>
-      <c r="L82" s="98">
+      <c r="I82" s="108"/>
+      <c r="J82" s="108"/>
+      <c r="K82" s="108"/>
+      <c r="L82" s="106">
         <v>92.4</v>
       </c>
-      <c r="M82" s="98"/>
-      <c r="N82" s="98"/>
-      <c r="P82" s="97">
+      <c r="M82" s="106"/>
+      <c r="N82" s="106"/>
+      <c r="P82" s="107">
         <f t="shared" si="2"/>
         <v>7635</v>
       </c>
-      <c r="Q82" s="97"/>
-      <c r="R82" s="97"/>
-      <c r="S82" s="97"/>
-      <c r="T82" s="97"/>
-      <c r="U82" s="97">
+      <c r="Q82" s="107"/>
+      <c r="R82" s="107"/>
+      <c r="S82" s="107"/>
+      <c r="T82" s="107"/>
+      <c r="U82" s="107">
         <f t="shared" si="3"/>
         <v>1350</v>
       </c>
-      <c r="V82" s="97"/>
-      <c r="W82" s="97"/>
+      <c r="V82" s="107"/>
+      <c r="W82" s="107"/>
       <c r="X82" s="48"/>
       <c r="AL82" s="1"/>
       <c r="AM82" s="74"/>
@@ -11937,65 +11948,65 @@
       <c r="BU82" s="76"/>
     </row>
     <row r="83" spans="3:73" ht="20">
-      <c r="C83" s="92">
+      <c r="C83" s="108">
         <v>20</v>
       </c>
-      <c r="D83" s="92"/>
-      <c r="E83" s="92">
+      <c r="D83" s="108"/>
+      <c r="E83" s="108">
         <v>3</v>
       </c>
-      <c r="F83" s="92"/>
-      <c r="G83" s="92"/>
-      <c r="H83" s="92" t="s">
+      <c r="F83" s="108"/>
+      <c r="G83" s="108"/>
+      <c r="H83" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="I83" s="92"/>
-      <c r="J83" s="92"/>
-      <c r="K83" s="92"/>
-      <c r="L83" s="92">
+      <c r="I83" s="108"/>
+      <c r="J83" s="108"/>
+      <c r="K83" s="108"/>
+      <c r="L83" s="108">
         <v>93.23</v>
       </c>
-      <c r="M83" s="92"/>
-      <c r="N83" s="92"/>
-      <c r="P83" s="92">
+      <c r="M83" s="108"/>
+      <c r="N83" s="108"/>
+      <c r="P83" s="108">
         <f t="shared" si="2"/>
         <v>7500</v>
       </c>
-      <c r="Q83" s="92"/>
-      <c r="R83" s="92"/>
-      <c r="S83" s="92"/>
-      <c r="T83" s="92"/>
-      <c r="U83" s="97">
+      <c r="Q83" s="108"/>
+      <c r="R83" s="108"/>
+      <c r="S83" s="108"/>
+      <c r="T83" s="108"/>
+      <c r="U83" s="107">
         <f t="shared" si="3"/>
         <v>5000</v>
       </c>
-      <c r="V83" s="97"/>
-      <c r="W83" s="97"/>
+      <c r="V83" s="107"/>
+      <c r="W83" s="107"/>
       <c r="X83" s="48"/>
       <c r="AL83" s="1"/>
       <c r="AM83" s="74"/>
-      <c r="AN83" s="96" t="s">
+      <c r="AN83" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="AO83" s="96"/>
-      <c r="AP83" s="96" t="s">
+      <c r="AO83" s="104"/>
+      <c r="AP83" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="AQ83" s="96"/>
-      <c r="AR83" s="96"/>
-      <c r="AS83" s="96" t="s">
+      <c r="AQ83" s="104"/>
+      <c r="AR83" s="104"/>
+      <c r="AS83" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="AT83" s="96"/>
-      <c r="AU83" s="96"/>
-      <c r="AV83" s="96"/>
-      <c r="AW83" s="96" t="s">
+      <c r="AT83" s="104"/>
+      <c r="AU83" s="104"/>
+      <c r="AV83" s="104"/>
+      <c r="AW83" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="AX83" s="96"/>
-      <c r="AY83" s="96"/>
-      <c r="AZ83" s="96"/>
-      <c r="BA83" s="96"/>
+      <c r="AX83" s="104"/>
+      <c r="AY83" s="104"/>
+      <c r="AZ83" s="104"/>
+      <c r="BA83" s="104"/>
       <c r="BB83" s="58" t="s">
         <v>25</v>
       </c>
@@ -12003,13 +12014,13 @@
       <c r="BD83" s="58"/>
       <c r="BE83" s="58"/>
       <c r="BF83" s="47"/>
-      <c r="BG83" s="96" t="s">
+      <c r="BG83" s="104" t="s">
         <v>28</v>
       </c>
-      <c r="BH83" s="96"/>
-      <c r="BI83" s="96"/>
-      <c r="BJ83" s="96"/>
-      <c r="BK83" s="96"/>
+      <c r="BH83" s="104"/>
+      <c r="BI83" s="104"/>
+      <c r="BJ83" s="104"/>
+      <c r="BK83" s="104"/>
       <c r="BL83" s="58" t="s">
         <v>26</v>
       </c>
@@ -12024,95 +12035,95 @@
       <c r="BU83" s="76"/>
     </row>
     <row r="84" spans="3:73" ht="20">
-      <c r="C84" s="92">
+      <c r="C84" s="108">
         <v>20</v>
       </c>
-      <c r="D84" s="92"/>
-      <c r="E84" s="92">
+      <c r="D84" s="108"/>
+      <c r="E84" s="108">
         <v>3</v>
       </c>
-      <c r="F84" s="92"/>
-      <c r="G84" s="92"/>
-      <c r="H84" s="92" t="s">
+      <c r="F84" s="108"/>
+      <c r="G84" s="108"/>
+      <c r="H84" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="I84" s="92"/>
-      <c r="J84" s="92"/>
-      <c r="K84" s="92"/>
-      <c r="L84" s="92">
+      <c r="I84" s="108"/>
+      <c r="J84" s="108"/>
+      <c r="K84" s="108"/>
+      <c r="L84" s="108">
         <v>92.73</v>
       </c>
-      <c r="M84" s="92"/>
-      <c r="N84" s="92"/>
-      <c r="P84" s="92">
+      <c r="M84" s="108"/>
+      <c r="N84" s="108"/>
+      <c r="P84" s="108">
         <f t="shared" si="2"/>
         <v>7500</v>
       </c>
-      <c r="Q84" s="92"/>
-      <c r="R84" s="92"/>
-      <c r="S84" s="92"/>
-      <c r="T84" s="92"/>
-      <c r="U84" s="97">
+      <c r="Q84" s="108"/>
+      <c r="R84" s="108"/>
+      <c r="S84" s="108"/>
+      <c r="T84" s="108"/>
+      <c r="U84" s="107">
         <f t="shared" si="3"/>
         <v>5000</v>
       </c>
-      <c r="V84" s="97"/>
-      <c r="W84" s="97"/>
+      <c r="V84" s="107"/>
+      <c r="W84" s="107"/>
       <c r="X84" s="48"/>
       <c r="AL84" s="1"/>
       <c r="AM84" s="74"/>
-      <c r="AN84" s="101">
+      <c r="AN84" s="97">
         <v>1</v>
       </c>
-      <c r="AO84" s="101"/>
-      <c r="AP84" s="101">
+      <c r="AO84" s="97"/>
+      <c r="AP84" s="97">
         <v>1</v>
       </c>
-      <c r="AQ84" s="101"/>
-      <c r="AR84" s="101"/>
-      <c r="AS84" s="101">
+      <c r="AQ84" s="97"/>
+      <c r="AR84" s="97"/>
+      <c r="AS84" s="97">
         <v>60</v>
       </c>
-      <c r="AT84" s="101"/>
-      <c r="AU84" s="101"/>
-      <c r="AV84" s="101"/>
-      <c r="AW84" s="102">
+      <c r="AT84" s="97"/>
+      <c r="AU84" s="97"/>
+      <c r="AV84" s="97"/>
+      <c r="AW84" s="99">
         <v>28</v>
       </c>
-      <c r="AX84" s="102"/>
+      <c r="AX84" s="99"/>
       <c r="AY84" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="AZ84" s="102">
+      <c r="AZ84" s="99">
         <v>28</v>
       </c>
-      <c r="BA84" s="102"/>
-      <c r="BB84" s="101">
+      <c r="BA84" s="99"/>
+      <c r="BB84" s="97">
         <f>AP84*AW84*AZ84</f>
         <v>784</v>
       </c>
-      <c r="BC84" s="101"/>
-      <c r="BD84" s="101"/>
-      <c r="BE84" s="101"/>
+      <c r="BC84" s="97"/>
+      <c r="BD84" s="97"/>
+      <c r="BE84" s="97"/>
       <c r="BF84" s="77"/>
-      <c r="BG84" s="102">
+      <c r="BG84" s="99">
         <v>30</v>
       </c>
-      <c r="BH84" s="102"/>
+      <c r="BH84" s="99"/>
       <c r="BI84" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="BJ84" s="102">
+      <c r="BJ84" s="99">
         <v>30</v>
       </c>
-      <c r="BK84" s="102"/>
-      <c r="BL84" s="101">
+      <c r="BK84" s="99"/>
+      <c r="BL84" s="97">
         <f>AS84*BG84*BJ84</f>
         <v>54000</v>
       </c>
-      <c r="BM84" s="101"/>
-      <c r="BN84" s="101"/>
-      <c r="BO84" s="101"/>
+      <c r="BM84" s="97"/>
+      <c r="BN84" s="97"/>
+      <c r="BO84" s="97"/>
       <c r="BP84" s="1"/>
       <c r="BQ84" s="1"/>
       <c r="BR84" s="63" t="s">
@@ -12123,389 +12134,389 @@
       <c r="BU84" s="76"/>
     </row>
     <row r="85" spans="3:73" ht="20">
-      <c r="C85" s="97">
+      <c r="C85" s="107">
         <v>20</v>
       </c>
-      <c r="D85" s="97"/>
-      <c r="E85" s="97">
+      <c r="D85" s="107"/>
+      <c r="E85" s="107">
         <v>5</v>
       </c>
-      <c r="F85" s="97"/>
-      <c r="G85" s="97"/>
-      <c r="H85" s="92" t="s">
+      <c r="F85" s="107"/>
+      <c r="G85" s="107"/>
+      <c r="H85" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="I85" s="92"/>
-      <c r="J85" s="92"/>
-      <c r="K85" s="92"/>
-      <c r="L85" s="97">
+      <c r="I85" s="108"/>
+      <c r="J85" s="108"/>
+      <c r="K85" s="108"/>
+      <c r="L85" s="107">
         <v>93.28</v>
       </c>
-      <c r="M85" s="97"/>
-      <c r="N85" s="97"/>
-      <c r="P85" s="97">
+      <c r="M85" s="107"/>
+      <c r="N85" s="107"/>
+      <c r="P85" s="107">
         <f t="shared" si="2"/>
         <v>7500</v>
       </c>
-      <c r="Q85" s="97"/>
-      <c r="R85" s="97"/>
-      <c r="S85" s="97"/>
-      <c r="T85" s="97"/>
-      <c r="U85" s="97">
+      <c r="Q85" s="107"/>
+      <c r="R85" s="107"/>
+      <c r="S85" s="107"/>
+      <c r="T85" s="107"/>
+      <c r="U85" s="107">
         <f t="shared" si="3"/>
         <v>1800</v>
       </c>
-      <c r="V85" s="97"/>
-      <c r="W85" s="97"/>
+      <c r="V85" s="107"/>
+      <c r="W85" s="107"/>
       <c r="X85" s="48"/>
       <c r="AL85" s="1"/>
       <c r="AM85" s="74"/>
-      <c r="AN85" s="108">
+      <c r="AN85" s="95">
         <v>2</v>
       </c>
-      <c r="AO85" s="108"/>
-      <c r="AP85" s="108">
+      <c r="AO85" s="95"/>
+      <c r="AP85" s="95">
         <v>60</v>
       </c>
-      <c r="AQ85" s="108"/>
-      <c r="AR85" s="108"/>
-      <c r="AS85" s="101">
+      <c r="AQ85" s="95"/>
+      <c r="AR85" s="95"/>
+      <c r="AS85" s="97">
         <v>60</v>
       </c>
-      <c r="AT85" s="101"/>
-      <c r="AU85" s="101"/>
-      <c r="AV85" s="101"/>
-      <c r="AW85" s="109">
+      <c r="AT85" s="97"/>
+      <c r="AU85" s="97"/>
+      <c r="AV85" s="97"/>
+      <c r="AW85" s="98">
         <v>30</v>
       </c>
-      <c r="AX85" s="109"/>
+      <c r="AX85" s="98"/>
       <c r="AY85" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="AZ85" s="109">
+      <c r="AZ85" s="98">
         <v>30</v>
       </c>
-      <c r="BA85" s="109"/>
-      <c r="BB85" s="101">
+      <c r="BA85" s="98"/>
+      <c r="BB85" s="97">
         <f>AP85*AW85*AZ85</f>
         <v>54000</v>
       </c>
-      <c r="BC85" s="101"/>
-      <c r="BD85" s="101"/>
-      <c r="BE85" s="101"/>
+      <c r="BC85" s="97"/>
+      <c r="BD85" s="97"/>
+      <c r="BE85" s="97"/>
       <c r="BF85" s="77"/>
-      <c r="BG85" s="102">
+      <c r="BG85" s="99">
         <v>16</v>
       </c>
-      <c r="BH85" s="102"/>
+      <c r="BH85" s="99"/>
       <c r="BI85" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="BJ85" s="102">
+      <c r="BJ85" s="99">
         <v>16</v>
       </c>
-      <c r="BK85" s="102"/>
-      <c r="BL85" s="101">
+      <c r="BK85" s="99"/>
+      <c r="BL85" s="97">
         <f>AS85*BG85*BJ85</f>
         <v>15360</v>
       </c>
-      <c r="BM85" s="101"/>
-      <c r="BN85" s="101"/>
-      <c r="BO85" s="101"/>
+      <c r="BM85" s="97"/>
+      <c r="BN85" s="97"/>
+      <c r="BO85" s="97"/>
       <c r="BP85" s="1"/>
       <c r="BQ85" s="1"/>
       <c r="BR85" s="63" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="BS85" s="1"/>
       <c r="BT85" s="1"/>
       <c r="BU85" s="76"/>
     </row>
     <row r="86" spans="3:73" ht="20">
-      <c r="C86" s="92">
+      <c r="C86" s="108">
         <v>25</v>
       </c>
-      <c r="D86" s="92"/>
-      <c r="E86" s="92">
+      <c r="D86" s="108"/>
+      <c r="E86" s="108">
         <v>5</v>
       </c>
-      <c r="F86" s="92"/>
-      <c r="G86" s="92"/>
-      <c r="H86" s="92" t="s">
+      <c r="F86" s="108"/>
+      <c r="G86" s="108"/>
+      <c r="H86" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="I86" s="92"/>
-      <c r="J86" s="92"/>
-      <c r="K86" s="92"/>
-      <c r="L86" s="92">
+      <c r="I86" s="108"/>
+      <c r="J86" s="108"/>
+      <c r="K86" s="108"/>
+      <c r="L86" s="108">
         <v>92.43</v>
       </c>
-      <c r="M86" s="92"/>
-      <c r="N86" s="92"/>
-      <c r="P86" s="92">
+      <c r="M86" s="108"/>
+      <c r="N86" s="108"/>
+      <c r="P86" s="108">
         <f t="shared" si="2"/>
         <v>7315</v>
       </c>
-      <c r="Q86" s="92"/>
-      <c r="R86" s="92"/>
-      <c r="S86" s="92"/>
-      <c r="T86" s="92"/>
-      <c r="U86" s="97">
+      <c r="Q86" s="108"/>
+      <c r="R86" s="108"/>
+      <c r="S86" s="108"/>
+      <c r="T86" s="108"/>
+      <c r="U86" s="107">
         <f t="shared" si="3"/>
         <v>2250</v>
       </c>
-      <c r="V86" s="97"/>
-      <c r="W86" s="97"/>
+      <c r="V86" s="107"/>
+      <c r="W86" s="107"/>
       <c r="X86" s="48"/>
       <c r="AM86" s="74"/>
-      <c r="AN86" s="108">
+      <c r="AN86" s="95">
         <v>3</v>
       </c>
-      <c r="AO86" s="108"/>
-      <c r="AP86" s="108">
+      <c r="AO86" s="95"/>
+      <c r="AP86" s="95">
         <v>60</v>
       </c>
-      <c r="AQ86" s="108"/>
-      <c r="AR86" s="108"/>
-      <c r="AS86" s="101">
+      <c r="AQ86" s="95"/>
+      <c r="AR86" s="95"/>
+      <c r="AS86" s="97">
         <v>56</v>
       </c>
-      <c r="AT86" s="101"/>
-      <c r="AU86" s="101"/>
-      <c r="AV86" s="101"/>
-      <c r="AW86" s="109">
+      <c r="AT86" s="97"/>
+      <c r="AU86" s="97"/>
+      <c r="AV86" s="97"/>
+      <c r="AW86" s="98">
         <v>16</v>
       </c>
-      <c r="AX86" s="109"/>
+      <c r="AX86" s="98"/>
       <c r="AY86" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="AZ86" s="109">
+      <c r="AZ86" s="98">
         <v>16</v>
       </c>
-      <c r="BA86" s="109"/>
-      <c r="BB86" s="101">
+      <c r="BA86" s="98"/>
+      <c r="BB86" s="97">
         <f>AP86*AW86*AZ86</f>
         <v>15360</v>
       </c>
-      <c r="BC86" s="101"/>
-      <c r="BD86" s="101"/>
-      <c r="BE86" s="101"/>
+      <c r="BC86" s="97"/>
+      <c r="BD86" s="97"/>
+      <c r="BE86" s="97"/>
       <c r="BF86" s="77"/>
-      <c r="BG86" s="102">
-        <v>16</v>
-      </c>
-      <c r="BH86" s="102"/>
+      <c r="BG86" s="99">
+        <v>8</v>
+      </c>
+      <c r="BH86" s="99"/>
       <c r="BI86" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="BJ86" s="102">
-        <v>16</v>
-      </c>
-      <c r="BK86" s="102"/>
-      <c r="BL86" s="101">
+      <c r="BJ86" s="99">
+        <v>8</v>
+      </c>
+      <c r="BK86" s="99"/>
+      <c r="BL86" s="97">
         <f>AS86*BG86*BJ86</f>
-        <v>14336</v>
-      </c>
-      <c r="BM86" s="101"/>
-      <c r="BN86" s="101"/>
-      <c r="BO86" s="101"/>
+        <v>3584</v>
+      </c>
+      <c r="BM86" s="97"/>
+      <c r="BN86" s="97"/>
+      <c r="BO86" s="97"/>
       <c r="BP86" s="1"/>
       <c r="BQ86" s="1"/>
       <c r="BR86" s="63" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="BS86" s="1"/>
       <c r="BT86" s="1"/>
       <c r="BU86" s="76"/>
     </row>
     <row r="87" spans="3:73" ht="20">
-      <c r="C87" s="92">
+      <c r="C87" s="108">
         <v>30</v>
       </c>
-      <c r="D87" s="92"/>
-      <c r="E87" s="92">
+      <c r="D87" s="108"/>
+      <c r="E87" s="108">
         <v>5</v>
       </c>
-      <c r="F87" s="92"/>
-      <c r="G87" s="92"/>
-      <c r="H87" s="92" t="s">
+      <c r="F87" s="108"/>
+      <c r="G87" s="108"/>
+      <c r="H87" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="I87" s="92"/>
-      <c r="J87" s="92"/>
-      <c r="K87" s="92"/>
-      <c r="L87" s="92">
+      <c r="I87" s="108"/>
+      <c r="J87" s="108"/>
+      <c r="K87" s="108"/>
+      <c r="L87" s="108">
         <v>93.13</v>
       </c>
-      <c r="M87" s="92"/>
-      <c r="N87" s="92"/>
-      <c r="P87" s="92">
+      <c r="M87" s="108"/>
+      <c r="N87" s="108"/>
+      <c r="P87" s="108">
         <f t="shared" si="2"/>
         <v>7080</v>
       </c>
-      <c r="Q87" s="92"/>
-      <c r="R87" s="92"/>
-      <c r="S87" s="92"/>
-      <c r="T87" s="92"/>
-      <c r="U87" s="97">
+      <c r="Q87" s="108"/>
+      <c r="R87" s="108"/>
+      <c r="S87" s="108"/>
+      <c r="T87" s="108"/>
+      <c r="U87" s="107">
         <f t="shared" si="3"/>
         <v>2700</v>
       </c>
-      <c r="V87" s="97"/>
-      <c r="W87" s="97"/>
+      <c r="V87" s="107"/>
+      <c r="W87" s="107"/>
       <c r="X87" s="48"/>
       <c r="AM87" s="74"/>
-      <c r="AN87" s="108">
+      <c r="AN87" s="95">
         <v>4</v>
       </c>
-      <c r="AO87" s="108"/>
-      <c r="AP87" s="108">
+      <c r="AO87" s="95"/>
+      <c r="AP87" s="95">
         <v>56</v>
       </c>
-      <c r="AQ87" s="108"/>
-      <c r="AR87" s="108"/>
-      <c r="AS87" s="101">
+      <c r="AQ87" s="95"/>
+      <c r="AR87" s="95"/>
+      <c r="AS87" s="97">
         <v>12</v>
       </c>
-      <c r="AT87" s="101"/>
-      <c r="AU87" s="101"/>
-      <c r="AV87" s="101"/>
-      <c r="AW87" s="109">
-        <v>16</v>
-      </c>
-      <c r="AX87" s="109"/>
+      <c r="AT87" s="97"/>
+      <c r="AU87" s="97"/>
+      <c r="AV87" s="97"/>
+      <c r="AW87" s="98">
+        <v>8</v>
+      </c>
+      <c r="AX87" s="98"/>
       <c r="AY87" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="AZ87" s="109">
-        <v>16</v>
-      </c>
-      <c r="BA87" s="109"/>
-      <c r="BB87" s="101">
+      <c r="AZ87" s="98">
+        <v>8</v>
+      </c>
+      <c r="BA87" s="98"/>
+      <c r="BB87" s="97">
         <f>AP87*AW87*AZ87</f>
-        <v>14336</v>
-      </c>
-      <c r="BC87" s="101"/>
-      <c r="BD87" s="101"/>
-      <c r="BE87" s="101"/>
+        <v>3584</v>
+      </c>
+      <c r="BC87" s="97"/>
+      <c r="BD87" s="97"/>
+      <c r="BE87" s="97"/>
       <c r="BF87" s="77"/>
-      <c r="BG87" s="102">
+      <c r="BG87" s="99">
         <v>4</v>
       </c>
-      <c r="BH87" s="102"/>
+      <c r="BH87" s="99"/>
       <c r="BI87" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="BJ87" s="102">
+      <c r="BJ87" s="99">
         <v>4</v>
       </c>
-      <c r="BK87" s="102"/>
-      <c r="BL87" s="101">
+      <c r="BK87" s="99"/>
+      <c r="BL87" s="97">
         <f>AS87*BG87*BJ87</f>
         <v>192</v>
       </c>
-      <c r="BM87" s="101"/>
-      <c r="BN87" s="101"/>
-      <c r="BO87" s="101"/>
+      <c r="BM87" s="97"/>
+      <c r="BN87" s="97"/>
+      <c r="BO87" s="97"/>
       <c r="BP87" s="1"/>
       <c r="BQ87" s="1"/>
       <c r="BR87" s="63" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="BS87" s="1"/>
       <c r="BT87" s="1"/>
       <c r="BU87" s="76"/>
     </row>
     <row r="88" spans="3:73" ht="20">
-      <c r="C88" s="92">
+      <c r="C88" s="108">
         <v>34</v>
       </c>
-      <c r="D88" s="92"/>
-      <c r="E88" s="92">
+      <c r="D88" s="108"/>
+      <c r="E88" s="108">
         <v>5</v>
       </c>
-      <c r="F88" s="92"/>
-      <c r="G88" s="92"/>
-      <c r="H88" s="92" t="s">
+      <c r="F88" s="108"/>
+      <c r="G88" s="108"/>
+      <c r="H88" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="I88" s="92"/>
-      <c r="J88" s="92"/>
-      <c r="K88" s="92"/>
-      <c r="L88" s="92">
+      <c r="I88" s="108"/>
+      <c r="J88" s="108"/>
+      <c r="K88" s="108"/>
+      <c r="L88" s="108">
         <v>92.82</v>
       </c>
-      <c r="M88" s="92"/>
-      <c r="N88" s="92"/>
-      <c r="P88" s="92">
+      <c r="M88" s="108"/>
+      <c r="N88" s="108"/>
+      <c r="P88" s="108">
         <f t="shared" si="2"/>
         <v>6856</v>
       </c>
-      <c r="Q88" s="92"/>
-      <c r="R88" s="92"/>
-      <c r="S88" s="92"/>
-      <c r="T88" s="92"/>
-      <c r="U88" s="97">
+      <c r="Q88" s="108"/>
+      <c r="R88" s="108"/>
+      <c r="S88" s="108"/>
+      <c r="T88" s="108"/>
+      <c r="U88" s="107">
         <f t="shared" si="3"/>
         <v>3060</v>
       </c>
-      <c r="V88" s="97"/>
-      <c r="W88" s="97"/>
+      <c r="V88" s="107"/>
+      <c r="W88" s="107"/>
       <c r="X88" s="48"/>
       <c r="AM88" s="74"/>
-      <c r="AN88" s="107">
+      <c r="AN88" s="102">
         <v>5</v>
       </c>
-      <c r="AO88" s="107"/>
-      <c r="AP88" s="107">
+      <c r="AO88" s="102"/>
+      <c r="AP88" s="102">
         <v>12</v>
       </c>
-      <c r="AQ88" s="107"/>
-      <c r="AR88" s="107"/>
-      <c r="AS88" s="105">
+      <c r="AQ88" s="102"/>
+      <c r="AR88" s="102"/>
+      <c r="AS88" s="101">
         <v>10</v>
       </c>
-      <c r="AT88" s="105"/>
-      <c r="AU88" s="105"/>
-      <c r="AV88" s="105"/>
-      <c r="AW88" s="104">
+      <c r="AT88" s="101"/>
+      <c r="AU88" s="101"/>
+      <c r="AV88" s="101"/>
+      <c r="AW88" s="103">
         <v>4</v>
       </c>
-      <c r="AX88" s="104"/>
+      <c r="AX88" s="103"/>
       <c r="AY88" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AZ88" s="104">
+      <c r="AZ88" s="103">
         <v>4</v>
       </c>
-      <c r="BA88" s="104"/>
-      <c r="BB88" s="105">
+      <c r="BA88" s="103"/>
+      <c r="BB88" s="101">
         <f>AP88*AW88*AZ88</f>
         <v>192</v>
       </c>
-      <c r="BC88" s="105"/>
-      <c r="BD88" s="105"/>
-      <c r="BE88" s="105"/>
+      <c r="BC88" s="101"/>
+      <c r="BD88" s="101"/>
+      <c r="BE88" s="101"/>
       <c r="BF88" s="66"/>
-      <c r="BG88" s="106">
+      <c r="BG88" s="100">
         <v>1</v>
       </c>
-      <c r="BH88" s="106"/>
+      <c r="BH88" s="100"/>
       <c r="BI88" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="BJ88" s="106">
+      <c r="BJ88" s="100">
         <v>10</v>
       </c>
-      <c r="BK88" s="106"/>
-      <c r="BL88" s="105">
+      <c r="BK88" s="100"/>
+      <c r="BL88" s="101">
         <f>AS88*BG88*BJ88</f>
         <v>100</v>
       </c>
-      <c r="BM88" s="105"/>
-      <c r="BN88" s="105"/>
-      <c r="BO88" s="105"/>
+      <c r="BM88" s="101"/>
+      <c r="BN88" s="101"/>
+      <c r="BO88" s="101"/>
       <c r="BP88" s="68"/>
       <c r="BQ88" s="68"/>
       <c r="BR88" s="69" t="s">
@@ -12556,237 +12567,114 @@
       <c r="BU89" s="81"/>
     </row>
     <row r="90" spans="3:73" ht="20">
-      <c r="C90" s="99">
+      <c r="C90" s="109">
         <v>12</v>
       </c>
-      <c r="D90" s="99"/>
-      <c r="E90" s="99">
+      <c r="D90" s="109"/>
+      <c r="E90" s="109">
         <v>4</v>
       </c>
-      <c r="F90" s="99"/>
-      <c r="G90" s="99"/>
-      <c r="H90" s="99" t="s">
+      <c r="F90" s="109"/>
+      <c r="G90" s="109"/>
+      <c r="H90" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="I90" s="99"/>
-      <c r="J90" s="99"/>
-      <c r="K90" s="99"/>
-      <c r="L90" s="100">
+      <c r="I90" s="109"/>
+      <c r="J90" s="109"/>
+      <c r="K90" s="109"/>
+      <c r="L90" s="110">
         <v>93.1</v>
       </c>
-      <c r="M90" s="100"/>
-      <c r="N90" s="100"/>
+      <c r="M90" s="110"/>
+      <c r="N90" s="110"/>
       <c r="O90" s="70"/>
-      <c r="P90" s="99">
+      <c r="P90" s="109">
         <f>61*60+60*(68-C90)+(68-C90)*C90</f>
         <v>7692</v>
       </c>
-      <c r="Q90" s="99"/>
-      <c r="R90" s="99"/>
-      <c r="S90" s="99"/>
-      <c r="T90" s="99"/>
-      <c r="U90" s="99">
+      <c r="Q90" s="109"/>
+      <c r="R90" s="109"/>
+      <c r="S90" s="109"/>
+      <c r="T90" s="109"/>
+      <c r="U90" s="109">
         <f>C90*FLOOR(IF(E90=3,15,16)/E90,1)^2*10</f>
         <v>1920</v>
       </c>
-      <c r="V90" s="99"/>
-      <c r="W90" s="99"/>
+      <c r="V90" s="109"/>
+      <c r="W90" s="109"/>
     </row>
     <row r="91" spans="3:73" ht="20">
-      <c r="C91" s="99">
+      <c r="C91" s="109">
         <v>12</v>
       </c>
-      <c r="D91" s="99"/>
-      <c r="E91" s="99">
+      <c r="D91" s="109"/>
+      <c r="E91" s="109">
         <v>4</v>
       </c>
-      <c r="F91" s="99"/>
-      <c r="G91" s="99"/>
-      <c r="H91" s="99" t="s">
+      <c r="F91" s="109"/>
+      <c r="G91" s="109"/>
+      <c r="H91" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="I91" s="99"/>
-      <c r="J91" s="99"/>
-      <c r="K91" s="99"/>
-      <c r="L91" s="100">
+      <c r="I91" s="109"/>
+      <c r="J91" s="109"/>
+      <c r="K91" s="109"/>
+      <c r="L91" s="110">
         <v>93.07</v>
       </c>
-      <c r="M91" s="100"/>
-      <c r="N91" s="100"/>
+      <c r="M91" s="110"/>
+      <c r="N91" s="110"/>
       <c r="O91" s="70"/>
-      <c r="P91" s="99">
+      <c r="P91" s="109">
         <f>61*60+60*(68-C91)+(68-C91)*C91</f>
         <v>7692</v>
       </c>
-      <c r="Q91" s="99"/>
-      <c r="R91" s="99"/>
-      <c r="S91" s="99"/>
-      <c r="T91" s="99"/>
-      <c r="U91" s="99">
+      <c r="Q91" s="109"/>
+      <c r="R91" s="109"/>
+      <c r="S91" s="109"/>
+      <c r="T91" s="109"/>
+      <c r="U91" s="109">
         <f>C91*FLOOR(IF(E91=3,15,16)/E91,1)^2*10</f>
         <v>1920</v>
       </c>
-      <c r="V91" s="99"/>
-      <c r="W91" s="99"/>
+      <c r="V91" s="109"/>
+      <c r="W91" s="109"/>
     </row>
   </sheetData>
   <mergeCells count="214">
-    <mergeCell ref="AN86:AO86"/>
-    <mergeCell ref="AP86:AR86"/>
-    <mergeCell ref="EB34:EB35"/>
-    <mergeCell ref="AN87:AO87"/>
-    <mergeCell ref="AP87:AR87"/>
-    <mergeCell ref="AS87:AV87"/>
-    <mergeCell ref="AW87:AX87"/>
-    <mergeCell ref="AZ87:BA87"/>
-    <mergeCell ref="BB87:BE87"/>
-    <mergeCell ref="BG87:BH87"/>
-    <mergeCell ref="BJ87:BK87"/>
-    <mergeCell ref="BL87:BO87"/>
-    <mergeCell ref="BG88:BH88"/>
-    <mergeCell ref="BJ88:BK88"/>
-    <mergeCell ref="BL88:BO88"/>
-    <mergeCell ref="AN88:AO88"/>
-    <mergeCell ref="AP88:AR88"/>
-    <mergeCell ref="AS88:AV88"/>
-    <mergeCell ref="AW88:AX88"/>
-    <mergeCell ref="AZ88:BA88"/>
-    <mergeCell ref="BB88:BE88"/>
-    <mergeCell ref="AS86:AV86"/>
-    <mergeCell ref="AW86:AX86"/>
-    <mergeCell ref="AZ86:BA86"/>
-    <mergeCell ref="BB86:BE86"/>
-    <mergeCell ref="BG86:BH86"/>
-    <mergeCell ref="BJ86:BK86"/>
-    <mergeCell ref="BG84:BH84"/>
-    <mergeCell ref="BJ84:BK84"/>
-    <mergeCell ref="BL84:BO84"/>
-    <mergeCell ref="BL86:BO86"/>
-    <mergeCell ref="BJ85:BK85"/>
-    <mergeCell ref="BL85:BO85"/>
-    <mergeCell ref="AN85:AO85"/>
-    <mergeCell ref="AP85:AR85"/>
-    <mergeCell ref="AS85:AV85"/>
-    <mergeCell ref="AW85:AX85"/>
-    <mergeCell ref="AZ85:BA85"/>
-    <mergeCell ref="BB85:BE85"/>
-    <mergeCell ref="BG85:BH85"/>
-    <mergeCell ref="AN84:AO84"/>
-    <mergeCell ref="AP84:AR84"/>
-    <mergeCell ref="AS84:AV84"/>
-    <mergeCell ref="AW84:AX84"/>
-    <mergeCell ref="AZ84:BA84"/>
-    <mergeCell ref="BB84:BE84"/>
-    <mergeCell ref="AN83:AO83"/>
-    <mergeCell ref="AP83:AR83"/>
-    <mergeCell ref="AS83:AV83"/>
-    <mergeCell ref="AW83:BA83"/>
-    <mergeCell ref="BG83:BK83"/>
-    <mergeCell ref="BG77:BH77"/>
-    <mergeCell ref="BJ77:BK77"/>
-    <mergeCell ref="BL77:BO77"/>
-    <mergeCell ref="AZ78:BA78"/>
-    <mergeCell ref="BB78:BE78"/>
-    <mergeCell ref="BG78:BH78"/>
-    <mergeCell ref="BJ78:BK78"/>
-    <mergeCell ref="BL78:BO78"/>
-    <mergeCell ref="AW77:AX77"/>
-    <mergeCell ref="AW78:AX78"/>
-    <mergeCell ref="AZ77:BA77"/>
-    <mergeCell ref="BB77:BE77"/>
-    <mergeCell ref="AN78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
-    <mergeCell ref="AS78:AV78"/>
-    <mergeCell ref="AW74:AX74"/>
-    <mergeCell ref="AZ76:BA76"/>
-    <mergeCell ref="BB76:BE76"/>
-    <mergeCell ref="BG76:BH76"/>
-    <mergeCell ref="BJ76:BK76"/>
-    <mergeCell ref="BL76:BO76"/>
-    <mergeCell ref="BG73:BK73"/>
-    <mergeCell ref="BG74:BH74"/>
-    <mergeCell ref="BJ74:BK74"/>
-    <mergeCell ref="BL74:BO74"/>
-    <mergeCell ref="BB75:BE75"/>
-    <mergeCell ref="BG75:BH75"/>
-    <mergeCell ref="BJ75:BK75"/>
-    <mergeCell ref="BL75:BO75"/>
-    <mergeCell ref="AZ74:BA74"/>
-    <mergeCell ref="AZ75:BA75"/>
-    <mergeCell ref="AW73:BA73"/>
-    <mergeCell ref="BB74:BE74"/>
-    <mergeCell ref="AW75:AX75"/>
-    <mergeCell ref="AW76:AX76"/>
-    <mergeCell ref="AN73:AO73"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="AS73:AV73"/>
-    <mergeCell ref="AN74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
-    <mergeCell ref="AS74:AV74"/>
-    <mergeCell ref="L79:N79"/>
-    <mergeCell ref="P79:T79"/>
-    <mergeCell ref="U79:W79"/>
-    <mergeCell ref="U76:W76"/>
-    <mergeCell ref="AP76:AR76"/>
-    <mergeCell ref="AS76:AV76"/>
-    <mergeCell ref="AN77:AO77"/>
-    <mergeCell ref="AP77:AR77"/>
-    <mergeCell ref="AS77:AV77"/>
-    <mergeCell ref="AN75:AO75"/>
-    <mergeCell ref="AP75:AR75"/>
-    <mergeCell ref="AS75:AV75"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="E91:G91"/>
-    <mergeCell ref="H91:K91"/>
-    <mergeCell ref="L91:N91"/>
-    <mergeCell ref="P91:T91"/>
-    <mergeCell ref="U91:W91"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="E90:G90"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:N90"/>
-    <mergeCell ref="P90:T90"/>
-    <mergeCell ref="U90:W90"/>
-    <mergeCell ref="H88:K88"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="H76:K76"/>
-    <mergeCell ref="L76:N76"/>
-    <mergeCell ref="P76:T76"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="E79:G79"/>
-    <mergeCell ref="H80:K80"/>
-    <mergeCell ref="H81:K81"/>
-    <mergeCell ref="H82:K82"/>
-    <mergeCell ref="H83:K83"/>
-    <mergeCell ref="H85:K85"/>
-    <mergeCell ref="H86:K86"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="E81:G81"/>
-    <mergeCell ref="L81:N81"/>
-    <mergeCell ref="P81:T81"/>
-    <mergeCell ref="U81:W81"/>
-    <mergeCell ref="H79:K79"/>
-    <mergeCell ref="H87:K87"/>
-    <mergeCell ref="H73:K73"/>
-    <mergeCell ref="H74:K74"/>
-    <mergeCell ref="H75:K75"/>
-    <mergeCell ref="H77:K77"/>
-    <mergeCell ref="U82:W82"/>
-    <mergeCell ref="U83:W83"/>
-    <mergeCell ref="U85:W85"/>
-    <mergeCell ref="U86:W86"/>
-    <mergeCell ref="U87:W87"/>
-    <mergeCell ref="L82:N82"/>
-    <mergeCell ref="P82:T82"/>
-    <mergeCell ref="L85:N85"/>
-    <mergeCell ref="L83:N83"/>
-    <mergeCell ref="L87:N87"/>
-    <mergeCell ref="L86:N86"/>
-    <mergeCell ref="H84:K84"/>
-    <mergeCell ref="L84:N84"/>
-    <mergeCell ref="P84:T84"/>
-    <mergeCell ref="U84:W84"/>
+    <mergeCell ref="A3:A18"/>
+    <mergeCell ref="A19:A34"/>
+    <mergeCell ref="A51:A66"/>
+    <mergeCell ref="A35:A50"/>
+    <mergeCell ref="L88:N88"/>
+    <mergeCell ref="E83:G83"/>
+    <mergeCell ref="DT70:DU70"/>
+    <mergeCell ref="AF70:AG70"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="L74:N74"/>
+    <mergeCell ref="L73:N73"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="P73:T73"/>
+    <mergeCell ref="P74:T74"/>
+    <mergeCell ref="P83:T83"/>
+    <mergeCell ref="P85:T85"/>
+    <mergeCell ref="P86:T86"/>
+    <mergeCell ref="L77:N77"/>
+    <mergeCell ref="H78:K78"/>
+    <mergeCell ref="E85:G85"/>
+    <mergeCell ref="E86:G86"/>
+    <mergeCell ref="E87:G87"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="E84:G84"/>
     <mergeCell ref="U88:W88"/>
     <mergeCell ref="U74:W74"/>
     <mergeCell ref="U75:W75"/>
@@ -12811,40 +12699,163 @@
     <mergeCell ref="P88:T88"/>
     <mergeCell ref="C82:D82"/>
     <mergeCell ref="E82:G82"/>
+    <mergeCell ref="U81:W81"/>
+    <mergeCell ref="H79:K79"/>
+    <mergeCell ref="H87:K87"/>
+    <mergeCell ref="H73:K73"/>
+    <mergeCell ref="H74:K74"/>
+    <mergeCell ref="H75:K75"/>
+    <mergeCell ref="H77:K77"/>
+    <mergeCell ref="U82:W82"/>
+    <mergeCell ref="U83:W83"/>
+    <mergeCell ref="U85:W85"/>
+    <mergeCell ref="U86:W86"/>
+    <mergeCell ref="U87:W87"/>
+    <mergeCell ref="L82:N82"/>
+    <mergeCell ref="P82:T82"/>
+    <mergeCell ref="L85:N85"/>
+    <mergeCell ref="L83:N83"/>
+    <mergeCell ref="L87:N87"/>
+    <mergeCell ref="L86:N86"/>
+    <mergeCell ref="H84:K84"/>
+    <mergeCell ref="L84:N84"/>
+    <mergeCell ref="P84:T84"/>
+    <mergeCell ref="U84:W84"/>
+    <mergeCell ref="H88:K88"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="H76:K76"/>
+    <mergeCell ref="L76:N76"/>
+    <mergeCell ref="P76:T76"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="H80:K80"/>
+    <mergeCell ref="H81:K81"/>
+    <mergeCell ref="H82:K82"/>
+    <mergeCell ref="H83:K83"/>
+    <mergeCell ref="H85:K85"/>
+    <mergeCell ref="H86:K86"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="E81:G81"/>
+    <mergeCell ref="L81:N81"/>
+    <mergeCell ref="P81:T81"/>
     <mergeCell ref="E88:G88"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="E77:G77"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="E84:G84"/>
-    <mergeCell ref="A3:A18"/>
-    <mergeCell ref="A19:A34"/>
-    <mergeCell ref="A51:A66"/>
-    <mergeCell ref="A35:A50"/>
-    <mergeCell ref="L88:N88"/>
-    <mergeCell ref="E83:G83"/>
-    <mergeCell ref="DT70:DU70"/>
-    <mergeCell ref="AF70:AG70"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="L74:N74"/>
-    <mergeCell ref="L73:N73"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="P73:T73"/>
-    <mergeCell ref="P74:T74"/>
-    <mergeCell ref="P83:T83"/>
-    <mergeCell ref="P85:T85"/>
-    <mergeCell ref="P86:T86"/>
-    <mergeCell ref="L77:N77"/>
-    <mergeCell ref="H78:K78"/>
-    <mergeCell ref="E85:G85"/>
-    <mergeCell ref="E86:G86"/>
-    <mergeCell ref="E87:G87"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="E91:G91"/>
+    <mergeCell ref="H91:K91"/>
+    <mergeCell ref="L91:N91"/>
+    <mergeCell ref="P91:T91"/>
+    <mergeCell ref="U91:W91"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="E90:G90"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:N90"/>
+    <mergeCell ref="P90:T90"/>
+    <mergeCell ref="U90:W90"/>
+    <mergeCell ref="AN73:AO73"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="AS73:AV73"/>
+    <mergeCell ref="AN74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AS74:AV74"/>
+    <mergeCell ref="L79:N79"/>
+    <mergeCell ref="P79:T79"/>
+    <mergeCell ref="U79:W79"/>
+    <mergeCell ref="U76:W76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AS76:AV76"/>
+    <mergeCell ref="AN77:AO77"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AS77:AV77"/>
+    <mergeCell ref="AN75:AO75"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AS75:AV75"/>
+    <mergeCell ref="AW74:AX74"/>
+    <mergeCell ref="AZ76:BA76"/>
+    <mergeCell ref="BB76:BE76"/>
+    <mergeCell ref="BG76:BH76"/>
+    <mergeCell ref="BJ76:BK76"/>
+    <mergeCell ref="BL76:BO76"/>
+    <mergeCell ref="BG73:BK73"/>
+    <mergeCell ref="BG74:BH74"/>
+    <mergeCell ref="BJ74:BK74"/>
+    <mergeCell ref="BL74:BO74"/>
+    <mergeCell ref="BB75:BE75"/>
+    <mergeCell ref="BG75:BH75"/>
+    <mergeCell ref="BJ75:BK75"/>
+    <mergeCell ref="BL75:BO75"/>
+    <mergeCell ref="AZ74:BA74"/>
+    <mergeCell ref="AZ75:BA75"/>
+    <mergeCell ref="AW73:BA73"/>
+    <mergeCell ref="BB74:BE74"/>
+    <mergeCell ref="AW75:AX75"/>
+    <mergeCell ref="AW76:AX76"/>
+    <mergeCell ref="AN83:AO83"/>
+    <mergeCell ref="AP83:AR83"/>
+    <mergeCell ref="AS83:AV83"/>
+    <mergeCell ref="AW83:BA83"/>
+    <mergeCell ref="BG83:BK83"/>
+    <mergeCell ref="BG77:BH77"/>
+    <mergeCell ref="BJ77:BK77"/>
+    <mergeCell ref="BL77:BO77"/>
+    <mergeCell ref="AZ78:BA78"/>
+    <mergeCell ref="BB78:BE78"/>
+    <mergeCell ref="BG78:BH78"/>
+    <mergeCell ref="BJ78:BK78"/>
+    <mergeCell ref="BL78:BO78"/>
+    <mergeCell ref="AW77:AX77"/>
+    <mergeCell ref="AW78:AX78"/>
+    <mergeCell ref="AZ77:BA77"/>
+    <mergeCell ref="BB77:BE77"/>
+    <mergeCell ref="AN78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AS78:AV78"/>
+    <mergeCell ref="AN85:AO85"/>
+    <mergeCell ref="AP85:AR85"/>
+    <mergeCell ref="AS85:AV85"/>
+    <mergeCell ref="AW85:AX85"/>
+    <mergeCell ref="AZ85:BA85"/>
+    <mergeCell ref="BB85:BE85"/>
+    <mergeCell ref="BG85:BH85"/>
+    <mergeCell ref="AN84:AO84"/>
+    <mergeCell ref="AP84:AR84"/>
+    <mergeCell ref="AS84:AV84"/>
+    <mergeCell ref="AW84:AX84"/>
+    <mergeCell ref="AZ84:BA84"/>
+    <mergeCell ref="BB84:BE84"/>
+    <mergeCell ref="BG88:BH88"/>
+    <mergeCell ref="BJ88:BK88"/>
+    <mergeCell ref="BL88:BO88"/>
+    <mergeCell ref="AN88:AO88"/>
+    <mergeCell ref="AP88:AR88"/>
+    <mergeCell ref="AS88:AV88"/>
+    <mergeCell ref="AW88:AX88"/>
+    <mergeCell ref="AZ88:BA88"/>
+    <mergeCell ref="BB88:BE88"/>
+    <mergeCell ref="AN86:AO86"/>
+    <mergeCell ref="AP86:AR86"/>
+    <mergeCell ref="EB34:EB35"/>
+    <mergeCell ref="AN87:AO87"/>
+    <mergeCell ref="AP87:AR87"/>
+    <mergeCell ref="AS87:AV87"/>
+    <mergeCell ref="AW87:AX87"/>
+    <mergeCell ref="AZ87:BA87"/>
+    <mergeCell ref="BB87:BE87"/>
+    <mergeCell ref="BG87:BH87"/>
+    <mergeCell ref="BJ87:BK87"/>
+    <mergeCell ref="BL87:BO87"/>
+    <mergeCell ref="AS86:AV86"/>
+    <mergeCell ref="AW86:AX86"/>
+    <mergeCell ref="AZ86:BA86"/>
+    <mergeCell ref="BB86:BE86"/>
+    <mergeCell ref="BG86:BH86"/>
+    <mergeCell ref="BJ86:BK86"/>
+    <mergeCell ref="BG84:BH84"/>
+    <mergeCell ref="BJ84:BK84"/>
+    <mergeCell ref="BL84:BO84"/>
+    <mergeCell ref="BL86:BO86"/>
+    <mergeCell ref="BJ85:BK85"/>
+    <mergeCell ref="BL85:BO85"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="47" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>